<commit_message>
Store Customer Data APIs
Update APIs to fix issues when storing FileContent into temp tables
</commit_message>
<xml_diff>
--- a/Code/Customer Data Upload Template.xlsx
+++ b/Code/Customer Data Upload Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B2516D-35CC-4A19-B959-E857F3D8BA0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C7526E-178A-4CE6-B8B0-695FFFE3C46A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,11 +244,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="000"/>
-    <numFmt numFmtId="165" formatCode="00"/>
-    <numFmt numFmtId="166" formatCode="0000"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -323,18 +318,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="]_x000d__x000a_Zoomed=1_x000d__x000a_Row=0_x000d__x000a_Column=0_x000d__x000a_Height=0_x000d__x000a_Width=0_x000d__x000a_FontName=FoxFont_x000d__x000a_FontStyle=0_x000d__x000a_FontSize=9_x000d__x000a_PrtFontName=FoxPrin" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -351,10 +343,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -685,25 +673,26 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1721,24 +1710,25 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2756,37 +2746,38 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3804,60 +3795,61 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="0" style="3" hidden="1"/>
+    <col min="16" max="16384" width="8.85546875" style="6" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2"/>
@@ -4876,61 +4868,62 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -5948,29 +5941,30 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -6990,169 +6984,169 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="52" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="52" width="5.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.85546875" style="6" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="1">
         <v>6.25E-2</v>
       </c>
-      <c r="F1" s="9">
+      <c r="F1" s="1">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="G1" s="9">
+      <c r="G1" s="1">
         <v>0.104166666666667</v>
       </c>
-      <c r="H1" s="9">
+      <c r="H1" s="1">
         <v>0.125</v>
       </c>
-      <c r="I1" s="9">
+      <c r="I1" s="1">
         <v>0.14583333333333301</v>
       </c>
-      <c r="J1" s="9">
+      <c r="J1" s="1">
         <v>0.16666666666666599</v>
       </c>
-      <c r="K1" s="9">
+      <c r="K1" s="1">
         <v>0.1875</v>
       </c>
-      <c r="L1" s="9">
+      <c r="L1" s="1">
         <v>0.20833333333333301</v>
       </c>
-      <c r="M1" s="9">
+      <c r="M1" s="1">
         <v>0.22916666666666599</v>
       </c>
-      <c r="N1" s="9">
+      <c r="N1" s="1">
         <v>0.25</v>
       </c>
-      <c r="O1" s="9">
+      <c r="O1" s="1">
         <v>0.27083333333333298</v>
       </c>
-      <c r="P1" s="9">
+      <c r="P1" s="1">
         <v>0.29166666666666602</v>
       </c>
-      <c r="Q1" s="9">
+      <c r="Q1" s="1">
         <v>0.3125</v>
       </c>
-      <c r="R1" s="9">
+      <c r="R1" s="1">
         <v>0.33333333333333298</v>
       </c>
-      <c r="S1" s="9">
+      <c r="S1" s="1">
         <v>0.35416666666666602</v>
       </c>
-      <c r="T1" s="9">
+      <c r="T1" s="1">
         <v>0.375</v>
       </c>
-      <c r="U1" s="9">
+      <c r="U1" s="1">
         <v>0.39583333333333298</v>
       </c>
-      <c r="V1" s="9">
+      <c r="V1" s="1">
         <v>0.41666666666666602</v>
       </c>
-      <c r="W1" s="9">
+      <c r="W1" s="1">
         <v>0.4375</v>
       </c>
-      <c r="X1" s="9">
+      <c r="X1" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="Y1" s="9">
+      <c r="Y1" s="1">
         <v>0.47916666666666602</v>
       </c>
-      <c r="Z1" s="9">
+      <c r="Z1" s="1">
         <v>0.5</v>
       </c>
-      <c r="AA1" s="9">
+      <c r="AA1" s="1">
         <v>0.52083333333333304</v>
       </c>
-      <c r="AB1" s="9">
+      <c r="AB1" s="1">
         <v>0.54166666666666596</v>
       </c>
-      <c r="AC1" s="9">
+      <c r="AC1" s="1">
         <v>0.5625</v>
       </c>
-      <c r="AD1" s="9">
+      <c r="AD1" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="AE1" s="9">
+      <c r="AE1" s="1">
         <v>0.60416666666666596</v>
       </c>
-      <c r="AF1" s="9">
+      <c r="AF1" s="1">
         <v>0.625</v>
       </c>
-      <c r="AG1" s="9">
+      <c r="AG1" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="AH1" s="9">
+      <c r="AH1" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="AI1" s="9">
+      <c r="AI1" s="1">
         <v>0.6875</v>
       </c>
-      <c r="AJ1" s="9">
+      <c r="AJ1" s="1">
         <v>0.70833333333333304</v>
       </c>
-      <c r="AK1" s="9">
+      <c r="AK1" s="1">
         <v>0.72916666666666596</v>
       </c>
-      <c r="AL1" s="9">
+      <c r="AL1" s="1">
         <v>0.75</v>
       </c>
-      <c r="AM1" s="9">
+      <c r="AM1" s="1">
         <v>0.77083333333333304</v>
       </c>
-      <c r="AN1" s="9">
+      <c r="AN1" s="1">
         <v>0.79166666666666596</v>
       </c>
-      <c r="AO1" s="9">
+      <c r="AO1" s="1">
         <v>0.8125</v>
       </c>
-      <c r="AP1" s="9">
+      <c r="AP1" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="AQ1" s="9">
+      <c r="AQ1" s="1">
         <v>0.85416666666666596</v>
       </c>
-      <c r="AR1" s="9">
+      <c r="AR1" s="1">
         <v>0.875</v>
       </c>
-      <c r="AS1" s="9">
+      <c r="AS1" s="1">
         <v>0.89583333333333304</v>
       </c>
-      <c r="AT1" s="9">
+      <c r="AT1" s="1">
         <v>0.91666666666666596</v>
       </c>
-      <c r="AU1" s="9">
+      <c r="AU1" s="1">
         <v>0.9375</v>
       </c>
-      <c r="AV1" s="9">
+      <c r="AV1" s="1">
         <v>0.95833333333333304</v>
       </c>
-      <c r="AW1" s="9">
+      <c r="AW1" s="1">
         <v>0.97916666666666596</v>
       </c>
-      <c r="AX1" s="9">
+      <c r="AX1" s="1">
         <v>1</v>
       </c>
-      <c r="AY1" s="9">
+      <c r="AY1" s="1">
         <v>6.3194444444444442E-2</v>
       </c>
-      <c r="AZ1" s="9">
+      <c r="AZ1" s="1">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -7172,29 +7166,30 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8212,169 +8207,169 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="52" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="52" width="5.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.85546875" style="6" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="1">
         <v>6.25E-2</v>
       </c>
-      <c r="F1" s="9">
+      <c r="F1" s="1">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="G1" s="9">
+      <c r="G1" s="1">
         <v>0.104166666666667</v>
       </c>
-      <c r="H1" s="9">
+      <c r="H1" s="1">
         <v>0.125</v>
       </c>
-      <c r="I1" s="9">
+      <c r="I1" s="1">
         <v>0.14583333333333301</v>
       </c>
-      <c r="J1" s="9">
+      <c r="J1" s="1">
         <v>0.16666666666666599</v>
       </c>
-      <c r="K1" s="9">
+      <c r="K1" s="1">
         <v>0.1875</v>
       </c>
-      <c r="L1" s="9">
+      <c r="L1" s="1">
         <v>0.20833333333333301</v>
       </c>
-      <c r="M1" s="9">
+      <c r="M1" s="1">
         <v>0.22916666666666599</v>
       </c>
-      <c r="N1" s="9">
+      <c r="N1" s="1">
         <v>0.25</v>
       </c>
-      <c r="O1" s="9">
+      <c r="O1" s="1">
         <v>0.27083333333333298</v>
       </c>
-      <c r="P1" s="9">
+      <c r="P1" s="1">
         <v>0.29166666666666602</v>
       </c>
-      <c r="Q1" s="9">
+      <c r="Q1" s="1">
         <v>0.3125</v>
       </c>
-      <c r="R1" s="9">
+      <c r="R1" s="1">
         <v>0.33333333333333298</v>
       </c>
-      <c r="S1" s="9">
+      <c r="S1" s="1">
         <v>0.35416666666666602</v>
       </c>
-      <c r="T1" s="9">
+      <c r="T1" s="1">
         <v>0.375</v>
       </c>
-      <c r="U1" s="9">
+      <c r="U1" s="1">
         <v>0.39583333333333298</v>
       </c>
-      <c r="V1" s="9">
+      <c r="V1" s="1">
         <v>0.41666666666666602</v>
       </c>
-      <c r="W1" s="9">
+      <c r="W1" s="1">
         <v>0.4375</v>
       </c>
-      <c r="X1" s="9">
+      <c r="X1" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="Y1" s="9">
+      <c r="Y1" s="1">
         <v>0.47916666666666602</v>
       </c>
-      <c r="Z1" s="9">
+      <c r="Z1" s="1">
         <v>0.5</v>
       </c>
-      <c r="AA1" s="9">
+      <c r="AA1" s="1">
         <v>0.52083333333333304</v>
       </c>
-      <c r="AB1" s="9">
+      <c r="AB1" s="1">
         <v>0.54166666666666596</v>
       </c>
-      <c r="AC1" s="9">
+      <c r="AC1" s="1">
         <v>0.5625</v>
       </c>
-      <c r="AD1" s="9">
+      <c r="AD1" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="AE1" s="9">
+      <c r="AE1" s="1">
         <v>0.60416666666666596</v>
       </c>
-      <c r="AF1" s="9">
+      <c r="AF1" s="1">
         <v>0.625</v>
       </c>
-      <c r="AG1" s="9">
+      <c r="AG1" s="1">
         <v>0.64583333333333304</v>
       </c>
-      <c r="AH1" s="9">
+      <c r="AH1" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="AI1" s="9">
+      <c r="AI1" s="1">
         <v>0.6875</v>
       </c>
-      <c r="AJ1" s="9">
+      <c r="AJ1" s="1">
         <v>0.70833333333333304</v>
       </c>
-      <c r="AK1" s="9">
+      <c r="AK1" s="1">
         <v>0.72916666666666596</v>
       </c>
-      <c r="AL1" s="9">
+      <c r="AL1" s="1">
         <v>0.75</v>
       </c>
-      <c r="AM1" s="9">
+      <c r="AM1" s="1">
         <v>0.77083333333333304</v>
       </c>
-      <c r="AN1" s="9">
+      <c r="AN1" s="1">
         <v>0.79166666666666596</v>
       </c>
-      <c r="AO1" s="9">
+      <c r="AO1" s="1">
         <v>0.8125</v>
       </c>
-      <c r="AP1" s="9">
+      <c r="AP1" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="AQ1" s="9">
+      <c r="AQ1" s="1">
         <v>0.85416666666666596</v>
       </c>
-      <c r="AR1" s="9">
+      <c r="AR1" s="1">
         <v>0.875</v>
       </c>
-      <c r="AS1" s="9">
+      <c r="AS1" s="1">
         <v>0.89583333333333304</v>
       </c>
-      <c r="AT1" s="9">
+      <c r="AT1" s="1">
         <v>0.91666666666666596</v>
       </c>
-      <c r="AU1" s="9">
+      <c r="AU1" s="1">
         <v>0.9375</v>
       </c>
-      <c r="AV1" s="9">
+      <c r="AV1" s="1">
         <v>0.95833333333333304</v>
       </c>
-      <c r="AW1" s="9">
+      <c r="AW1" s="1">
         <v>0.97916666666666596</v>
       </c>
-      <c r="AX1" s="9">
+      <c r="AX1" s="1">
         <v>1</v>
       </c>
-      <c r="AY1" s="9">
+      <c r="AY1" s="1">
         <v>6.3194444444444442E-2</v>
       </c>
-      <c r="AZ1" s="9">
+      <c r="AZ1" s="1">
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
@@ -8394,77 +8389,78 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.28515625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -9476,7 +9472,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38228543-4DF3-482D-9DFD-988E8DB0F6D8}">
-  <dimension ref="A1:N1001"/>
+  <dimension ref="A1:S1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -9484,67 +9480,68 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="12.42578125" style="3" hidden="1"/>
+    <col min="19" max="19" width="13.5703125" style="3" hidden="1"/>
+    <col min="20" max="16384" width="9.28515625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="7" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MPRN Daily Usage Data
Changes to allow commit of Daily Usage for MPRNs
</commit_message>
<xml_diff>
--- a/Code/Customer Data Upload Template.xlsx
+++ b/Code/Customer Data Upload Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950055F9-982B-4C9E-93FA-8051D7EA3E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625C952B-01B3-4243-A1C4-C11E113B60AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" tabRatio="796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" tabRatio="796" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="15" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet name="Meters" sheetId="9" r:id="rId3"/>
     <sheet name="SubMeters" sheetId="7" r:id="rId4"/>
     <sheet name="Meter HH Data" sheetId="4" r:id="rId5"/>
-    <sheet name="Meter Exemptions" sheetId="11" r:id="rId6"/>
-    <sheet name="SubMeter HH Data" sheetId="8" r:id="rId7"/>
-    <sheet name="Fixed Contracts" sheetId="12" r:id="rId8"/>
-    <sheet name="Flex Contracts" sheetId="13" r:id="rId9"/>
-    <sheet name="Flex Reference Volumes" sheetId="14" r:id="rId10"/>
-    <sheet name="Flex Trades" sheetId="17" r:id="rId11"/>
+    <sheet name="MPRN Daily Data" sheetId="18" r:id="rId6"/>
+    <sheet name="Meter Exemptions" sheetId="11" r:id="rId7"/>
+    <sheet name="SubMeter HH Data" sheetId="8" r:id="rId8"/>
+    <sheet name="Fixed Contracts" sheetId="12" r:id="rId9"/>
+    <sheet name="Flex Contracts" sheetId="13" r:id="rId10"/>
+    <sheet name="Flex Reference Volumes" sheetId="14" r:id="rId11"/>
+    <sheet name="Flex Trades" sheetId="17" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>MTC</t>
   </si>
@@ -239,6 +240,12 @@
   <si>
     <t>Meter Serial Number</t>
   </si>
+  <si>
+    <t>MPRN</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
 </sst>
 </file>
 
@@ -319,7 +326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -328,6 +335,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="]_x000d__x000a_Zoomed=1_x000d__x000a_Row=0_x000d__x000a_Column=0_x000d__x000a_Height=0_x000d__x000a_Width=0_x000d__x000a_FontName=FoxFont_x000d__x000a_FontStyle=0_x000d__x000a_FontSize=9_x000d__x000a_PrtFontName=FoxPrin" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1703,6 +1712,1086 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38228543-4DF3-482D-9DFD-988E8DB0F6D8}">
+  <dimension ref="A1:S1001"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="12.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.28515625" style="3" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2"/>
+    <row r="17" x14ac:dyDescent="0.2"/>
+    <row r="18" x14ac:dyDescent="0.2"/>
+    <row r="19" x14ac:dyDescent="0.2"/>
+    <row r="20" x14ac:dyDescent="0.2"/>
+    <row r="21" x14ac:dyDescent="0.2"/>
+    <row r="22" x14ac:dyDescent="0.2"/>
+    <row r="23" x14ac:dyDescent="0.2"/>
+    <row r="24" x14ac:dyDescent="0.2"/>
+    <row r="25" x14ac:dyDescent="0.2"/>
+    <row r="26" x14ac:dyDescent="0.2"/>
+    <row r="27" x14ac:dyDescent="0.2"/>
+    <row r="28" x14ac:dyDescent="0.2"/>
+    <row r="29" x14ac:dyDescent="0.2"/>
+    <row r="30" x14ac:dyDescent="0.2"/>
+    <row r="31" x14ac:dyDescent="0.2"/>
+    <row r="32" x14ac:dyDescent="0.2"/>
+    <row r="33" x14ac:dyDescent="0.2"/>
+    <row r="34" x14ac:dyDescent="0.2"/>
+    <row r="35" x14ac:dyDescent="0.2"/>
+    <row r="36" x14ac:dyDescent="0.2"/>
+    <row r="37" x14ac:dyDescent="0.2"/>
+    <row r="38" x14ac:dyDescent="0.2"/>
+    <row r="39" x14ac:dyDescent="0.2"/>
+    <row r="40" x14ac:dyDescent="0.2"/>
+    <row r="41" x14ac:dyDescent="0.2"/>
+    <row r="42" x14ac:dyDescent="0.2"/>
+    <row r="43" x14ac:dyDescent="0.2"/>
+    <row r="44" x14ac:dyDescent="0.2"/>
+    <row r="45" x14ac:dyDescent="0.2"/>
+    <row r="46" x14ac:dyDescent="0.2"/>
+    <row r="47" x14ac:dyDescent="0.2"/>
+    <row r="48" x14ac:dyDescent="0.2"/>
+    <row r="49" x14ac:dyDescent="0.2"/>
+    <row r="50" x14ac:dyDescent="0.2"/>
+    <row r="51" x14ac:dyDescent="0.2"/>
+    <row r="52" x14ac:dyDescent="0.2"/>
+    <row r="53" x14ac:dyDescent="0.2"/>
+    <row r="54" x14ac:dyDescent="0.2"/>
+    <row r="55" x14ac:dyDescent="0.2"/>
+    <row r="56" x14ac:dyDescent="0.2"/>
+    <row r="57" x14ac:dyDescent="0.2"/>
+    <row r="58" x14ac:dyDescent="0.2"/>
+    <row r="59" x14ac:dyDescent="0.2"/>
+    <row r="60" x14ac:dyDescent="0.2"/>
+    <row r="61" x14ac:dyDescent="0.2"/>
+    <row r="62" x14ac:dyDescent="0.2"/>
+    <row r="63" x14ac:dyDescent="0.2"/>
+    <row r="64" x14ac:dyDescent="0.2"/>
+    <row r="65" x14ac:dyDescent="0.2"/>
+    <row r="66" x14ac:dyDescent="0.2"/>
+    <row r="67" x14ac:dyDescent="0.2"/>
+    <row r="68" x14ac:dyDescent="0.2"/>
+    <row r="69" x14ac:dyDescent="0.2"/>
+    <row r="70" x14ac:dyDescent="0.2"/>
+    <row r="71" x14ac:dyDescent="0.2"/>
+    <row r="72" x14ac:dyDescent="0.2"/>
+    <row r="73" x14ac:dyDescent="0.2"/>
+    <row r="74" x14ac:dyDescent="0.2"/>
+    <row r="75" x14ac:dyDescent="0.2"/>
+    <row r="76" x14ac:dyDescent="0.2"/>
+    <row r="77" x14ac:dyDescent="0.2"/>
+    <row r="78" x14ac:dyDescent="0.2"/>
+    <row r="79" x14ac:dyDescent="0.2"/>
+    <row r="80" x14ac:dyDescent="0.2"/>
+    <row r="81" x14ac:dyDescent="0.2"/>
+    <row r="82" x14ac:dyDescent="0.2"/>
+    <row r="83" x14ac:dyDescent="0.2"/>
+    <row r="84" x14ac:dyDescent="0.2"/>
+    <row r="85" x14ac:dyDescent="0.2"/>
+    <row r="86" x14ac:dyDescent="0.2"/>
+    <row r="87" x14ac:dyDescent="0.2"/>
+    <row r="88" x14ac:dyDescent="0.2"/>
+    <row r="89" x14ac:dyDescent="0.2"/>
+    <row r="90" x14ac:dyDescent="0.2"/>
+    <row r="91" x14ac:dyDescent="0.2"/>
+    <row r="92" x14ac:dyDescent="0.2"/>
+    <row r="93" x14ac:dyDescent="0.2"/>
+    <row r="94" x14ac:dyDescent="0.2"/>
+    <row r="95" x14ac:dyDescent="0.2"/>
+    <row r="96" x14ac:dyDescent="0.2"/>
+    <row r="97" x14ac:dyDescent="0.2"/>
+    <row r="98" x14ac:dyDescent="0.2"/>
+    <row r="99" x14ac:dyDescent="0.2"/>
+    <row r="100" x14ac:dyDescent="0.2"/>
+    <row r="101" x14ac:dyDescent="0.2"/>
+    <row r="102" x14ac:dyDescent="0.2"/>
+    <row r="103" x14ac:dyDescent="0.2"/>
+    <row r="104" x14ac:dyDescent="0.2"/>
+    <row r="105" x14ac:dyDescent="0.2"/>
+    <row r="106" x14ac:dyDescent="0.2"/>
+    <row r="107" x14ac:dyDescent="0.2"/>
+    <row r="108" x14ac:dyDescent="0.2"/>
+    <row r="109" x14ac:dyDescent="0.2"/>
+    <row r="110" x14ac:dyDescent="0.2"/>
+    <row r="111" x14ac:dyDescent="0.2"/>
+    <row r="112" x14ac:dyDescent="0.2"/>
+    <row r="113" x14ac:dyDescent="0.2"/>
+    <row r="114" x14ac:dyDescent="0.2"/>
+    <row r="115" x14ac:dyDescent="0.2"/>
+    <row r="116" x14ac:dyDescent="0.2"/>
+    <row r="117" x14ac:dyDescent="0.2"/>
+    <row r="118" x14ac:dyDescent="0.2"/>
+    <row r="119" x14ac:dyDescent="0.2"/>
+    <row r="120" x14ac:dyDescent="0.2"/>
+    <row r="121" x14ac:dyDescent="0.2"/>
+    <row r="122" x14ac:dyDescent="0.2"/>
+    <row r="123" x14ac:dyDescent="0.2"/>
+    <row r="124" x14ac:dyDescent="0.2"/>
+    <row r="125" x14ac:dyDescent="0.2"/>
+    <row r="126" x14ac:dyDescent="0.2"/>
+    <row r="127" x14ac:dyDescent="0.2"/>
+    <row r="128" x14ac:dyDescent="0.2"/>
+    <row r="129" x14ac:dyDescent="0.2"/>
+    <row r="130" x14ac:dyDescent="0.2"/>
+    <row r="131" x14ac:dyDescent="0.2"/>
+    <row r="132" x14ac:dyDescent="0.2"/>
+    <row r="133" x14ac:dyDescent="0.2"/>
+    <row r="134" x14ac:dyDescent="0.2"/>
+    <row r="135" x14ac:dyDescent="0.2"/>
+    <row r="136" x14ac:dyDescent="0.2"/>
+    <row r="137" x14ac:dyDescent="0.2"/>
+    <row r="138" x14ac:dyDescent="0.2"/>
+    <row r="139" x14ac:dyDescent="0.2"/>
+    <row r="140" x14ac:dyDescent="0.2"/>
+    <row r="141" x14ac:dyDescent="0.2"/>
+    <row r="142" x14ac:dyDescent="0.2"/>
+    <row r="143" x14ac:dyDescent="0.2"/>
+    <row r="144" x14ac:dyDescent="0.2"/>
+    <row r="145" x14ac:dyDescent="0.2"/>
+    <row r="146" x14ac:dyDescent="0.2"/>
+    <row r="147" x14ac:dyDescent="0.2"/>
+    <row r="148" x14ac:dyDescent="0.2"/>
+    <row r="149" x14ac:dyDescent="0.2"/>
+    <row r="150" x14ac:dyDescent="0.2"/>
+    <row r="151" x14ac:dyDescent="0.2"/>
+    <row r="152" x14ac:dyDescent="0.2"/>
+    <row r="153" x14ac:dyDescent="0.2"/>
+    <row r="154" x14ac:dyDescent="0.2"/>
+    <row r="155" x14ac:dyDescent="0.2"/>
+    <row r="156" x14ac:dyDescent="0.2"/>
+    <row r="157" x14ac:dyDescent="0.2"/>
+    <row r="158" x14ac:dyDescent="0.2"/>
+    <row r="159" x14ac:dyDescent="0.2"/>
+    <row r="160" x14ac:dyDescent="0.2"/>
+    <row r="161" x14ac:dyDescent="0.2"/>
+    <row r="162" x14ac:dyDescent="0.2"/>
+    <row r="163" x14ac:dyDescent="0.2"/>
+    <row r="164" x14ac:dyDescent="0.2"/>
+    <row r="165" x14ac:dyDescent="0.2"/>
+    <row r="166" x14ac:dyDescent="0.2"/>
+    <row r="167" x14ac:dyDescent="0.2"/>
+    <row r="168" x14ac:dyDescent="0.2"/>
+    <row r="169" x14ac:dyDescent="0.2"/>
+    <row r="170" x14ac:dyDescent="0.2"/>
+    <row r="171" x14ac:dyDescent="0.2"/>
+    <row r="172" x14ac:dyDescent="0.2"/>
+    <row r="173" x14ac:dyDescent="0.2"/>
+    <row r="174" x14ac:dyDescent="0.2"/>
+    <row r="175" x14ac:dyDescent="0.2"/>
+    <row r="176" x14ac:dyDescent="0.2"/>
+    <row r="177" x14ac:dyDescent="0.2"/>
+    <row r="178" x14ac:dyDescent="0.2"/>
+    <row r="179" x14ac:dyDescent="0.2"/>
+    <row r="180" x14ac:dyDescent="0.2"/>
+    <row r="181" x14ac:dyDescent="0.2"/>
+    <row r="182" x14ac:dyDescent="0.2"/>
+    <row r="183" x14ac:dyDescent="0.2"/>
+    <row r="184" x14ac:dyDescent="0.2"/>
+    <row r="185" x14ac:dyDescent="0.2"/>
+    <row r="186" x14ac:dyDescent="0.2"/>
+    <row r="187" x14ac:dyDescent="0.2"/>
+    <row r="188" x14ac:dyDescent="0.2"/>
+    <row r="189" x14ac:dyDescent="0.2"/>
+    <row r="190" x14ac:dyDescent="0.2"/>
+    <row r="191" x14ac:dyDescent="0.2"/>
+    <row r="192" x14ac:dyDescent="0.2"/>
+    <row r="193" x14ac:dyDescent="0.2"/>
+    <row r="194" x14ac:dyDescent="0.2"/>
+    <row r="195" x14ac:dyDescent="0.2"/>
+    <row r="196" x14ac:dyDescent="0.2"/>
+    <row r="197" x14ac:dyDescent="0.2"/>
+    <row r="198" x14ac:dyDescent="0.2"/>
+    <row r="199" x14ac:dyDescent="0.2"/>
+    <row r="200" x14ac:dyDescent="0.2"/>
+    <row r="201" x14ac:dyDescent="0.2"/>
+    <row r="202" x14ac:dyDescent="0.2"/>
+    <row r="203" x14ac:dyDescent="0.2"/>
+    <row r="204" x14ac:dyDescent="0.2"/>
+    <row r="205" x14ac:dyDescent="0.2"/>
+    <row r="206" x14ac:dyDescent="0.2"/>
+    <row r="207" x14ac:dyDescent="0.2"/>
+    <row r="208" x14ac:dyDescent="0.2"/>
+    <row r="209" x14ac:dyDescent="0.2"/>
+    <row r="210" x14ac:dyDescent="0.2"/>
+    <row r="211" x14ac:dyDescent="0.2"/>
+    <row r="212" x14ac:dyDescent="0.2"/>
+    <row r="213" x14ac:dyDescent="0.2"/>
+    <row r="214" x14ac:dyDescent="0.2"/>
+    <row r="215" x14ac:dyDescent="0.2"/>
+    <row r="216" x14ac:dyDescent="0.2"/>
+    <row r="217" x14ac:dyDescent="0.2"/>
+    <row r="218" x14ac:dyDescent="0.2"/>
+    <row r="219" x14ac:dyDescent="0.2"/>
+    <row r="220" x14ac:dyDescent="0.2"/>
+    <row r="221" x14ac:dyDescent="0.2"/>
+    <row r="222" x14ac:dyDescent="0.2"/>
+    <row r="223" x14ac:dyDescent="0.2"/>
+    <row r="224" x14ac:dyDescent="0.2"/>
+    <row r="225" x14ac:dyDescent="0.2"/>
+    <row r="226" x14ac:dyDescent="0.2"/>
+    <row r="227" x14ac:dyDescent="0.2"/>
+    <row r="228" x14ac:dyDescent="0.2"/>
+    <row r="229" x14ac:dyDescent="0.2"/>
+    <row r="230" x14ac:dyDescent="0.2"/>
+    <row r="231" x14ac:dyDescent="0.2"/>
+    <row r="232" x14ac:dyDescent="0.2"/>
+    <row r="233" x14ac:dyDescent="0.2"/>
+    <row r="234" x14ac:dyDescent="0.2"/>
+    <row r="235" x14ac:dyDescent="0.2"/>
+    <row r="236" x14ac:dyDescent="0.2"/>
+    <row r="237" x14ac:dyDescent="0.2"/>
+    <row r="238" x14ac:dyDescent="0.2"/>
+    <row r="239" x14ac:dyDescent="0.2"/>
+    <row r="240" x14ac:dyDescent="0.2"/>
+    <row r="241" x14ac:dyDescent="0.2"/>
+    <row r="242" x14ac:dyDescent="0.2"/>
+    <row r="243" x14ac:dyDescent="0.2"/>
+    <row r="244" x14ac:dyDescent="0.2"/>
+    <row r="245" x14ac:dyDescent="0.2"/>
+    <row r="246" x14ac:dyDescent="0.2"/>
+    <row r="247" x14ac:dyDescent="0.2"/>
+    <row r="248" x14ac:dyDescent="0.2"/>
+    <row r="249" x14ac:dyDescent="0.2"/>
+    <row r="250" x14ac:dyDescent="0.2"/>
+    <row r="251" x14ac:dyDescent="0.2"/>
+    <row r="252" x14ac:dyDescent="0.2"/>
+    <row r="253" x14ac:dyDescent="0.2"/>
+    <row r="254" x14ac:dyDescent="0.2"/>
+    <row r="255" x14ac:dyDescent="0.2"/>
+    <row r="256" x14ac:dyDescent="0.2"/>
+    <row r="257" x14ac:dyDescent="0.2"/>
+    <row r="258" x14ac:dyDescent="0.2"/>
+    <row r="259" x14ac:dyDescent="0.2"/>
+    <row r="260" x14ac:dyDescent="0.2"/>
+    <row r="261" x14ac:dyDescent="0.2"/>
+    <row r="262" x14ac:dyDescent="0.2"/>
+    <row r="263" x14ac:dyDescent="0.2"/>
+    <row r="264" x14ac:dyDescent="0.2"/>
+    <row r="265" x14ac:dyDescent="0.2"/>
+    <row r="266" x14ac:dyDescent="0.2"/>
+    <row r="267" x14ac:dyDescent="0.2"/>
+    <row r="268" x14ac:dyDescent="0.2"/>
+    <row r="269" x14ac:dyDescent="0.2"/>
+    <row r="270" x14ac:dyDescent="0.2"/>
+    <row r="271" x14ac:dyDescent="0.2"/>
+    <row r="272" x14ac:dyDescent="0.2"/>
+    <row r="273" x14ac:dyDescent="0.2"/>
+    <row r="274" x14ac:dyDescent="0.2"/>
+    <row r="275" x14ac:dyDescent="0.2"/>
+    <row r="276" x14ac:dyDescent="0.2"/>
+    <row r="277" x14ac:dyDescent="0.2"/>
+    <row r="278" x14ac:dyDescent="0.2"/>
+    <row r="279" x14ac:dyDescent="0.2"/>
+    <row r="280" x14ac:dyDescent="0.2"/>
+    <row r="281" x14ac:dyDescent="0.2"/>
+    <row r="282" x14ac:dyDescent="0.2"/>
+    <row r="283" x14ac:dyDescent="0.2"/>
+    <row r="284" x14ac:dyDescent="0.2"/>
+    <row r="285" x14ac:dyDescent="0.2"/>
+    <row r="286" x14ac:dyDescent="0.2"/>
+    <row r="287" x14ac:dyDescent="0.2"/>
+    <row r="288" x14ac:dyDescent="0.2"/>
+    <row r="289" x14ac:dyDescent="0.2"/>
+    <row r="290" x14ac:dyDescent="0.2"/>
+    <row r="291" x14ac:dyDescent="0.2"/>
+    <row r="292" x14ac:dyDescent="0.2"/>
+    <row r="293" x14ac:dyDescent="0.2"/>
+    <row r="294" x14ac:dyDescent="0.2"/>
+    <row r="295" x14ac:dyDescent="0.2"/>
+    <row r="296" x14ac:dyDescent="0.2"/>
+    <row r="297" x14ac:dyDescent="0.2"/>
+    <row r="298" x14ac:dyDescent="0.2"/>
+    <row r="299" x14ac:dyDescent="0.2"/>
+    <row r="300" x14ac:dyDescent="0.2"/>
+    <row r="301" x14ac:dyDescent="0.2"/>
+    <row r="302" x14ac:dyDescent="0.2"/>
+    <row r="303" x14ac:dyDescent="0.2"/>
+    <row r="304" x14ac:dyDescent="0.2"/>
+    <row r="305" x14ac:dyDescent="0.2"/>
+    <row r="306" x14ac:dyDescent="0.2"/>
+    <row r="307" x14ac:dyDescent="0.2"/>
+    <row r="308" x14ac:dyDescent="0.2"/>
+    <row r="309" x14ac:dyDescent="0.2"/>
+    <row r="310" x14ac:dyDescent="0.2"/>
+    <row r="311" x14ac:dyDescent="0.2"/>
+    <row r="312" x14ac:dyDescent="0.2"/>
+    <row r="313" x14ac:dyDescent="0.2"/>
+    <row r="314" x14ac:dyDescent="0.2"/>
+    <row r="315" x14ac:dyDescent="0.2"/>
+    <row r="316" x14ac:dyDescent="0.2"/>
+    <row r="317" x14ac:dyDescent="0.2"/>
+    <row r="318" x14ac:dyDescent="0.2"/>
+    <row r="319" x14ac:dyDescent="0.2"/>
+    <row r="320" x14ac:dyDescent="0.2"/>
+    <row r="321" x14ac:dyDescent="0.2"/>
+    <row r="322" x14ac:dyDescent="0.2"/>
+    <row r="323" x14ac:dyDescent="0.2"/>
+    <row r="324" x14ac:dyDescent="0.2"/>
+    <row r="325" x14ac:dyDescent="0.2"/>
+    <row r="326" x14ac:dyDescent="0.2"/>
+    <row r="327" x14ac:dyDescent="0.2"/>
+    <row r="328" x14ac:dyDescent="0.2"/>
+    <row r="329" x14ac:dyDescent="0.2"/>
+    <row r="330" x14ac:dyDescent="0.2"/>
+    <row r="331" x14ac:dyDescent="0.2"/>
+    <row r="332" x14ac:dyDescent="0.2"/>
+    <row r="333" x14ac:dyDescent="0.2"/>
+    <row r="334" x14ac:dyDescent="0.2"/>
+    <row r="335" x14ac:dyDescent="0.2"/>
+    <row r="336" x14ac:dyDescent="0.2"/>
+    <row r="337" x14ac:dyDescent="0.2"/>
+    <row r="338" x14ac:dyDescent="0.2"/>
+    <row r="339" x14ac:dyDescent="0.2"/>
+    <row r="340" x14ac:dyDescent="0.2"/>
+    <row r="341" x14ac:dyDescent="0.2"/>
+    <row r="342" x14ac:dyDescent="0.2"/>
+    <row r="343" x14ac:dyDescent="0.2"/>
+    <row r="344" x14ac:dyDescent="0.2"/>
+    <row r="345" x14ac:dyDescent="0.2"/>
+    <row r="346" x14ac:dyDescent="0.2"/>
+    <row r="347" x14ac:dyDescent="0.2"/>
+    <row r="348" x14ac:dyDescent="0.2"/>
+    <row r="349" x14ac:dyDescent="0.2"/>
+    <row r="350" x14ac:dyDescent="0.2"/>
+    <row r="351" x14ac:dyDescent="0.2"/>
+    <row r="352" x14ac:dyDescent="0.2"/>
+    <row r="353" x14ac:dyDescent="0.2"/>
+    <row r="354" x14ac:dyDescent="0.2"/>
+    <row r="355" x14ac:dyDescent="0.2"/>
+    <row r="356" x14ac:dyDescent="0.2"/>
+    <row r="357" x14ac:dyDescent="0.2"/>
+    <row r="358" x14ac:dyDescent="0.2"/>
+    <row r="359" x14ac:dyDescent="0.2"/>
+    <row r="360" x14ac:dyDescent="0.2"/>
+    <row r="361" x14ac:dyDescent="0.2"/>
+    <row r="362" x14ac:dyDescent="0.2"/>
+    <row r="363" x14ac:dyDescent="0.2"/>
+    <row r="364" x14ac:dyDescent="0.2"/>
+    <row r="365" x14ac:dyDescent="0.2"/>
+    <row r="366" x14ac:dyDescent="0.2"/>
+    <row r="367" x14ac:dyDescent="0.2"/>
+    <row r="368" x14ac:dyDescent="0.2"/>
+    <row r="369" x14ac:dyDescent="0.2"/>
+    <row r="370" x14ac:dyDescent="0.2"/>
+    <row r="371" x14ac:dyDescent="0.2"/>
+    <row r="372" x14ac:dyDescent="0.2"/>
+    <row r="373" x14ac:dyDescent="0.2"/>
+    <row r="374" x14ac:dyDescent="0.2"/>
+    <row r="375" x14ac:dyDescent="0.2"/>
+    <row r="376" x14ac:dyDescent="0.2"/>
+    <row r="377" x14ac:dyDescent="0.2"/>
+    <row r="378" x14ac:dyDescent="0.2"/>
+    <row r="379" x14ac:dyDescent="0.2"/>
+    <row r="380" x14ac:dyDescent="0.2"/>
+    <row r="381" x14ac:dyDescent="0.2"/>
+    <row r="382" x14ac:dyDescent="0.2"/>
+    <row r="383" x14ac:dyDescent="0.2"/>
+    <row r="384" x14ac:dyDescent="0.2"/>
+    <row r="385" x14ac:dyDescent="0.2"/>
+    <row r="386" x14ac:dyDescent="0.2"/>
+    <row r="387" x14ac:dyDescent="0.2"/>
+    <row r="388" x14ac:dyDescent="0.2"/>
+    <row r="389" x14ac:dyDescent="0.2"/>
+    <row r="390" x14ac:dyDescent="0.2"/>
+    <row r="391" x14ac:dyDescent="0.2"/>
+    <row r="392" x14ac:dyDescent="0.2"/>
+    <row r="393" x14ac:dyDescent="0.2"/>
+    <row r="394" x14ac:dyDescent="0.2"/>
+    <row r="395" x14ac:dyDescent="0.2"/>
+    <row r="396" x14ac:dyDescent="0.2"/>
+    <row r="397" x14ac:dyDescent="0.2"/>
+    <row r="398" x14ac:dyDescent="0.2"/>
+    <row r="399" x14ac:dyDescent="0.2"/>
+    <row r="400" x14ac:dyDescent="0.2"/>
+    <row r="401" x14ac:dyDescent="0.2"/>
+    <row r="402" x14ac:dyDescent="0.2"/>
+    <row r="403" x14ac:dyDescent="0.2"/>
+    <row r="404" x14ac:dyDescent="0.2"/>
+    <row r="405" x14ac:dyDescent="0.2"/>
+    <row r="406" x14ac:dyDescent="0.2"/>
+    <row r="407" x14ac:dyDescent="0.2"/>
+    <row r="408" x14ac:dyDescent="0.2"/>
+    <row r="409" x14ac:dyDescent="0.2"/>
+    <row r="410" x14ac:dyDescent="0.2"/>
+    <row r="411" x14ac:dyDescent="0.2"/>
+    <row r="412" x14ac:dyDescent="0.2"/>
+    <row r="413" x14ac:dyDescent="0.2"/>
+    <row r="414" x14ac:dyDescent="0.2"/>
+    <row r="415" x14ac:dyDescent="0.2"/>
+    <row r="416" x14ac:dyDescent="0.2"/>
+    <row r="417" x14ac:dyDescent="0.2"/>
+    <row r="418" x14ac:dyDescent="0.2"/>
+    <row r="419" x14ac:dyDescent="0.2"/>
+    <row r="420" x14ac:dyDescent="0.2"/>
+    <row r="421" x14ac:dyDescent="0.2"/>
+    <row r="422" x14ac:dyDescent="0.2"/>
+    <row r="423" x14ac:dyDescent="0.2"/>
+    <row r="424" x14ac:dyDescent="0.2"/>
+    <row r="425" x14ac:dyDescent="0.2"/>
+    <row r="426" x14ac:dyDescent="0.2"/>
+    <row r="427" x14ac:dyDescent="0.2"/>
+    <row r="428" x14ac:dyDescent="0.2"/>
+    <row r="429" x14ac:dyDescent="0.2"/>
+    <row r="430" x14ac:dyDescent="0.2"/>
+    <row r="431" x14ac:dyDescent="0.2"/>
+    <row r="432" x14ac:dyDescent="0.2"/>
+    <row r="433" x14ac:dyDescent="0.2"/>
+    <row r="434" x14ac:dyDescent="0.2"/>
+    <row r="435" x14ac:dyDescent="0.2"/>
+    <row r="436" x14ac:dyDescent="0.2"/>
+    <row r="437" x14ac:dyDescent="0.2"/>
+    <row r="438" x14ac:dyDescent="0.2"/>
+    <row r="439" x14ac:dyDescent="0.2"/>
+    <row r="440" x14ac:dyDescent="0.2"/>
+    <row r="441" x14ac:dyDescent="0.2"/>
+    <row r="442" x14ac:dyDescent="0.2"/>
+    <row r="443" x14ac:dyDescent="0.2"/>
+    <row r="444" x14ac:dyDescent="0.2"/>
+    <row r="445" x14ac:dyDescent="0.2"/>
+    <row r="446" x14ac:dyDescent="0.2"/>
+    <row r="447" x14ac:dyDescent="0.2"/>
+    <row r="448" x14ac:dyDescent="0.2"/>
+    <row r="449" x14ac:dyDescent="0.2"/>
+    <row r="450" x14ac:dyDescent="0.2"/>
+    <row r="451" x14ac:dyDescent="0.2"/>
+    <row r="452" x14ac:dyDescent="0.2"/>
+    <row r="453" x14ac:dyDescent="0.2"/>
+    <row r="454" x14ac:dyDescent="0.2"/>
+    <row r="455" x14ac:dyDescent="0.2"/>
+    <row r="456" x14ac:dyDescent="0.2"/>
+    <row r="457" x14ac:dyDescent="0.2"/>
+    <row r="458" x14ac:dyDescent="0.2"/>
+    <row r="459" x14ac:dyDescent="0.2"/>
+    <row r="460" x14ac:dyDescent="0.2"/>
+    <row r="461" x14ac:dyDescent="0.2"/>
+    <row r="462" x14ac:dyDescent="0.2"/>
+    <row r="463" x14ac:dyDescent="0.2"/>
+    <row r="464" x14ac:dyDescent="0.2"/>
+    <row r="465" x14ac:dyDescent="0.2"/>
+    <row r="466" x14ac:dyDescent="0.2"/>
+    <row r="467" x14ac:dyDescent="0.2"/>
+    <row r="468" x14ac:dyDescent="0.2"/>
+    <row r="469" x14ac:dyDescent="0.2"/>
+    <row r="470" x14ac:dyDescent="0.2"/>
+    <row r="471" x14ac:dyDescent="0.2"/>
+    <row r="472" x14ac:dyDescent="0.2"/>
+    <row r="473" x14ac:dyDescent="0.2"/>
+    <row r="474" x14ac:dyDescent="0.2"/>
+    <row r="475" x14ac:dyDescent="0.2"/>
+    <row r="476" x14ac:dyDescent="0.2"/>
+    <row r="477" x14ac:dyDescent="0.2"/>
+    <row r="478" x14ac:dyDescent="0.2"/>
+    <row r="479" x14ac:dyDescent="0.2"/>
+    <row r="480" x14ac:dyDescent="0.2"/>
+    <row r="481" x14ac:dyDescent="0.2"/>
+    <row r="482" x14ac:dyDescent="0.2"/>
+    <row r="483" x14ac:dyDescent="0.2"/>
+    <row r="484" x14ac:dyDescent="0.2"/>
+    <row r="485" x14ac:dyDescent="0.2"/>
+    <row r="486" x14ac:dyDescent="0.2"/>
+    <row r="487" x14ac:dyDescent="0.2"/>
+    <row r="488" x14ac:dyDescent="0.2"/>
+    <row r="489" x14ac:dyDescent="0.2"/>
+    <row r="490" x14ac:dyDescent="0.2"/>
+    <row r="491" x14ac:dyDescent="0.2"/>
+    <row r="492" x14ac:dyDescent="0.2"/>
+    <row r="493" x14ac:dyDescent="0.2"/>
+    <row r="494" x14ac:dyDescent="0.2"/>
+    <row r="495" x14ac:dyDescent="0.2"/>
+    <row r="496" x14ac:dyDescent="0.2"/>
+    <row r="497" x14ac:dyDescent="0.2"/>
+    <row r="498" x14ac:dyDescent="0.2"/>
+    <row r="499" x14ac:dyDescent="0.2"/>
+    <row r="500" x14ac:dyDescent="0.2"/>
+    <row r="501" x14ac:dyDescent="0.2"/>
+    <row r="502" x14ac:dyDescent="0.2"/>
+    <row r="503" x14ac:dyDescent="0.2"/>
+    <row r="504" x14ac:dyDescent="0.2"/>
+    <row r="505" x14ac:dyDescent="0.2"/>
+    <row r="506" x14ac:dyDescent="0.2"/>
+    <row r="507" x14ac:dyDescent="0.2"/>
+    <row r="508" x14ac:dyDescent="0.2"/>
+    <row r="509" x14ac:dyDescent="0.2"/>
+    <row r="510" x14ac:dyDescent="0.2"/>
+    <row r="511" x14ac:dyDescent="0.2"/>
+    <row r="512" x14ac:dyDescent="0.2"/>
+    <row r="513" x14ac:dyDescent="0.2"/>
+    <row r="514" x14ac:dyDescent="0.2"/>
+    <row r="515" x14ac:dyDescent="0.2"/>
+    <row r="516" x14ac:dyDescent="0.2"/>
+    <row r="517" x14ac:dyDescent="0.2"/>
+    <row r="518" x14ac:dyDescent="0.2"/>
+    <row r="519" x14ac:dyDescent="0.2"/>
+    <row r="520" x14ac:dyDescent="0.2"/>
+    <row r="521" x14ac:dyDescent="0.2"/>
+    <row r="522" x14ac:dyDescent="0.2"/>
+    <row r="523" x14ac:dyDescent="0.2"/>
+    <row r="524" x14ac:dyDescent="0.2"/>
+    <row r="525" x14ac:dyDescent="0.2"/>
+    <row r="526" x14ac:dyDescent="0.2"/>
+    <row r="527" x14ac:dyDescent="0.2"/>
+    <row r="528" x14ac:dyDescent="0.2"/>
+    <row r="529" x14ac:dyDescent="0.2"/>
+    <row r="530" x14ac:dyDescent="0.2"/>
+    <row r="531" x14ac:dyDescent="0.2"/>
+    <row r="532" x14ac:dyDescent="0.2"/>
+    <row r="533" x14ac:dyDescent="0.2"/>
+    <row r="534" x14ac:dyDescent="0.2"/>
+    <row r="535" x14ac:dyDescent="0.2"/>
+    <row r="536" x14ac:dyDescent="0.2"/>
+    <row r="537" x14ac:dyDescent="0.2"/>
+    <row r="538" x14ac:dyDescent="0.2"/>
+    <row r="539" x14ac:dyDescent="0.2"/>
+    <row r="540" x14ac:dyDescent="0.2"/>
+    <row r="541" x14ac:dyDescent="0.2"/>
+    <row r="542" x14ac:dyDescent="0.2"/>
+    <row r="543" x14ac:dyDescent="0.2"/>
+    <row r="544" x14ac:dyDescent="0.2"/>
+    <row r="545" x14ac:dyDescent="0.2"/>
+    <row r="546" x14ac:dyDescent="0.2"/>
+    <row r="547" x14ac:dyDescent="0.2"/>
+    <row r="548" x14ac:dyDescent="0.2"/>
+    <row r="549" x14ac:dyDescent="0.2"/>
+    <row r="550" x14ac:dyDescent="0.2"/>
+    <row r="551" x14ac:dyDescent="0.2"/>
+    <row r="552" x14ac:dyDescent="0.2"/>
+    <row r="553" x14ac:dyDescent="0.2"/>
+    <row r="554" x14ac:dyDescent="0.2"/>
+    <row r="555" x14ac:dyDescent="0.2"/>
+    <row r="556" x14ac:dyDescent="0.2"/>
+    <row r="557" x14ac:dyDescent="0.2"/>
+    <row r="558" x14ac:dyDescent="0.2"/>
+    <row r="559" x14ac:dyDescent="0.2"/>
+    <row r="560" x14ac:dyDescent="0.2"/>
+    <row r="561" x14ac:dyDescent="0.2"/>
+    <row r="562" x14ac:dyDescent="0.2"/>
+    <row r="563" x14ac:dyDescent="0.2"/>
+    <row r="564" x14ac:dyDescent="0.2"/>
+    <row r="565" x14ac:dyDescent="0.2"/>
+    <row r="566" x14ac:dyDescent="0.2"/>
+    <row r="567" x14ac:dyDescent="0.2"/>
+    <row r="568" x14ac:dyDescent="0.2"/>
+    <row r="569" x14ac:dyDescent="0.2"/>
+    <row r="570" x14ac:dyDescent="0.2"/>
+    <row r="571" x14ac:dyDescent="0.2"/>
+    <row r="572" x14ac:dyDescent="0.2"/>
+    <row r="573" x14ac:dyDescent="0.2"/>
+    <row r="574" x14ac:dyDescent="0.2"/>
+    <row r="575" x14ac:dyDescent="0.2"/>
+    <row r="576" x14ac:dyDescent="0.2"/>
+    <row r="577" x14ac:dyDescent="0.2"/>
+    <row r="578" x14ac:dyDescent="0.2"/>
+    <row r="579" x14ac:dyDescent="0.2"/>
+    <row r="580" x14ac:dyDescent="0.2"/>
+    <row r="581" x14ac:dyDescent="0.2"/>
+    <row r="582" x14ac:dyDescent="0.2"/>
+    <row r="583" x14ac:dyDescent="0.2"/>
+    <row r="584" x14ac:dyDescent="0.2"/>
+    <row r="585" x14ac:dyDescent="0.2"/>
+    <row r="586" x14ac:dyDescent="0.2"/>
+    <row r="587" x14ac:dyDescent="0.2"/>
+    <row r="588" x14ac:dyDescent="0.2"/>
+    <row r="589" x14ac:dyDescent="0.2"/>
+    <row r="590" x14ac:dyDescent="0.2"/>
+    <row r="591" x14ac:dyDescent="0.2"/>
+    <row r="592" x14ac:dyDescent="0.2"/>
+    <row r="593" x14ac:dyDescent="0.2"/>
+    <row r="594" x14ac:dyDescent="0.2"/>
+    <row r="595" x14ac:dyDescent="0.2"/>
+    <row r="596" x14ac:dyDescent="0.2"/>
+    <row r="597" x14ac:dyDescent="0.2"/>
+    <row r="598" x14ac:dyDescent="0.2"/>
+    <row r="599" x14ac:dyDescent="0.2"/>
+    <row r="600" x14ac:dyDescent="0.2"/>
+    <row r="601" x14ac:dyDescent="0.2"/>
+    <row r="602" x14ac:dyDescent="0.2"/>
+    <row r="603" x14ac:dyDescent="0.2"/>
+    <row r="604" x14ac:dyDescent="0.2"/>
+    <row r="605" x14ac:dyDescent="0.2"/>
+    <row r="606" x14ac:dyDescent="0.2"/>
+    <row r="607" x14ac:dyDescent="0.2"/>
+    <row r="608" x14ac:dyDescent="0.2"/>
+    <row r="609" x14ac:dyDescent="0.2"/>
+    <row r="610" x14ac:dyDescent="0.2"/>
+    <row r="611" x14ac:dyDescent="0.2"/>
+    <row r="612" x14ac:dyDescent="0.2"/>
+    <row r="613" x14ac:dyDescent="0.2"/>
+    <row r="614" x14ac:dyDescent="0.2"/>
+    <row r="615" x14ac:dyDescent="0.2"/>
+    <row r="616" x14ac:dyDescent="0.2"/>
+    <row r="617" x14ac:dyDescent="0.2"/>
+    <row r="618" x14ac:dyDescent="0.2"/>
+    <row r="619" x14ac:dyDescent="0.2"/>
+    <row r="620" x14ac:dyDescent="0.2"/>
+    <row r="621" x14ac:dyDescent="0.2"/>
+    <row r="622" x14ac:dyDescent="0.2"/>
+    <row r="623" x14ac:dyDescent="0.2"/>
+    <row r="624" x14ac:dyDescent="0.2"/>
+    <row r="625" x14ac:dyDescent="0.2"/>
+    <row r="626" x14ac:dyDescent="0.2"/>
+    <row r="627" x14ac:dyDescent="0.2"/>
+    <row r="628" x14ac:dyDescent="0.2"/>
+    <row r="629" x14ac:dyDescent="0.2"/>
+    <row r="630" x14ac:dyDescent="0.2"/>
+    <row r="631" x14ac:dyDescent="0.2"/>
+    <row r="632" x14ac:dyDescent="0.2"/>
+    <row r="633" x14ac:dyDescent="0.2"/>
+    <row r="634" x14ac:dyDescent="0.2"/>
+    <row r="635" x14ac:dyDescent="0.2"/>
+    <row r="636" x14ac:dyDescent="0.2"/>
+    <row r="637" x14ac:dyDescent="0.2"/>
+    <row r="638" x14ac:dyDescent="0.2"/>
+    <row r="639" x14ac:dyDescent="0.2"/>
+    <row r="640" x14ac:dyDescent="0.2"/>
+    <row r="641" x14ac:dyDescent="0.2"/>
+    <row r="642" x14ac:dyDescent="0.2"/>
+    <row r="643" x14ac:dyDescent="0.2"/>
+    <row r="644" x14ac:dyDescent="0.2"/>
+    <row r="645" x14ac:dyDescent="0.2"/>
+    <row r="646" x14ac:dyDescent="0.2"/>
+    <row r="647" x14ac:dyDescent="0.2"/>
+    <row r="648" x14ac:dyDescent="0.2"/>
+    <row r="649" x14ac:dyDescent="0.2"/>
+    <row r="650" x14ac:dyDescent="0.2"/>
+    <row r="651" x14ac:dyDescent="0.2"/>
+    <row r="652" x14ac:dyDescent="0.2"/>
+    <row r="653" x14ac:dyDescent="0.2"/>
+    <row r="654" x14ac:dyDescent="0.2"/>
+    <row r="655" x14ac:dyDescent="0.2"/>
+    <row r="656" x14ac:dyDescent="0.2"/>
+    <row r="657" x14ac:dyDescent="0.2"/>
+    <row r="658" x14ac:dyDescent="0.2"/>
+    <row r="659" x14ac:dyDescent="0.2"/>
+    <row r="660" x14ac:dyDescent="0.2"/>
+    <row r="661" x14ac:dyDescent="0.2"/>
+    <row r="662" x14ac:dyDescent="0.2"/>
+    <row r="663" x14ac:dyDescent="0.2"/>
+    <row r="664" x14ac:dyDescent="0.2"/>
+    <row r="665" x14ac:dyDescent="0.2"/>
+    <row r="666" x14ac:dyDescent="0.2"/>
+    <row r="667" x14ac:dyDescent="0.2"/>
+    <row r="668" x14ac:dyDescent="0.2"/>
+    <row r="669" x14ac:dyDescent="0.2"/>
+    <row r="670" x14ac:dyDescent="0.2"/>
+    <row r="671" x14ac:dyDescent="0.2"/>
+    <row r="672" x14ac:dyDescent="0.2"/>
+    <row r="673" x14ac:dyDescent="0.2"/>
+    <row r="674" x14ac:dyDescent="0.2"/>
+    <row r="675" x14ac:dyDescent="0.2"/>
+    <row r="676" x14ac:dyDescent="0.2"/>
+    <row r="677" x14ac:dyDescent="0.2"/>
+    <row r="678" x14ac:dyDescent="0.2"/>
+    <row r="679" x14ac:dyDescent="0.2"/>
+    <row r="680" x14ac:dyDescent="0.2"/>
+    <row r="681" x14ac:dyDescent="0.2"/>
+    <row r="682" x14ac:dyDescent="0.2"/>
+    <row r="683" x14ac:dyDescent="0.2"/>
+    <row r="684" x14ac:dyDescent="0.2"/>
+    <row r="685" x14ac:dyDescent="0.2"/>
+    <row r="686" x14ac:dyDescent="0.2"/>
+    <row r="687" x14ac:dyDescent="0.2"/>
+    <row r="688" x14ac:dyDescent="0.2"/>
+    <row r="689" x14ac:dyDescent="0.2"/>
+    <row r="690" x14ac:dyDescent="0.2"/>
+    <row r="691" x14ac:dyDescent="0.2"/>
+    <row r="692" x14ac:dyDescent="0.2"/>
+    <row r="693" x14ac:dyDescent="0.2"/>
+    <row r="694" x14ac:dyDescent="0.2"/>
+    <row r="695" x14ac:dyDescent="0.2"/>
+    <row r="696" x14ac:dyDescent="0.2"/>
+    <row r="697" x14ac:dyDescent="0.2"/>
+    <row r="698" x14ac:dyDescent="0.2"/>
+    <row r="699" x14ac:dyDescent="0.2"/>
+    <row r="700" x14ac:dyDescent="0.2"/>
+    <row r="701" x14ac:dyDescent="0.2"/>
+    <row r="702" x14ac:dyDescent="0.2"/>
+    <row r="703" x14ac:dyDescent="0.2"/>
+    <row r="704" x14ac:dyDescent="0.2"/>
+    <row r="705" x14ac:dyDescent="0.2"/>
+    <row r="706" x14ac:dyDescent="0.2"/>
+    <row r="707" x14ac:dyDescent="0.2"/>
+    <row r="708" x14ac:dyDescent="0.2"/>
+    <row r="709" x14ac:dyDescent="0.2"/>
+    <row r="710" x14ac:dyDescent="0.2"/>
+    <row r="711" x14ac:dyDescent="0.2"/>
+    <row r="712" x14ac:dyDescent="0.2"/>
+    <row r="713" x14ac:dyDescent="0.2"/>
+    <row r="714" x14ac:dyDescent="0.2"/>
+    <row r="715" x14ac:dyDescent="0.2"/>
+    <row r="716" x14ac:dyDescent="0.2"/>
+    <row r="717" x14ac:dyDescent="0.2"/>
+    <row r="718" x14ac:dyDescent="0.2"/>
+    <row r="719" x14ac:dyDescent="0.2"/>
+    <row r="720" x14ac:dyDescent="0.2"/>
+    <row r="721" x14ac:dyDescent="0.2"/>
+    <row r="722" x14ac:dyDescent="0.2"/>
+    <row r="723" x14ac:dyDescent="0.2"/>
+    <row r="724" x14ac:dyDescent="0.2"/>
+    <row r="725" x14ac:dyDescent="0.2"/>
+    <row r="726" x14ac:dyDescent="0.2"/>
+    <row r="727" x14ac:dyDescent="0.2"/>
+    <row r="728" x14ac:dyDescent="0.2"/>
+    <row r="729" x14ac:dyDescent="0.2"/>
+    <row r="730" x14ac:dyDescent="0.2"/>
+    <row r="731" x14ac:dyDescent="0.2"/>
+    <row r="732" x14ac:dyDescent="0.2"/>
+    <row r="733" x14ac:dyDescent="0.2"/>
+    <row r="734" x14ac:dyDescent="0.2"/>
+    <row r="735" x14ac:dyDescent="0.2"/>
+    <row r="736" x14ac:dyDescent="0.2"/>
+    <row r="737" x14ac:dyDescent="0.2"/>
+    <row r="738" x14ac:dyDescent="0.2"/>
+    <row r="739" x14ac:dyDescent="0.2"/>
+    <row r="740" x14ac:dyDescent="0.2"/>
+    <row r="741" x14ac:dyDescent="0.2"/>
+    <row r="742" x14ac:dyDescent="0.2"/>
+    <row r="743" x14ac:dyDescent="0.2"/>
+    <row r="744" x14ac:dyDescent="0.2"/>
+    <row r="745" x14ac:dyDescent="0.2"/>
+    <row r="746" x14ac:dyDescent="0.2"/>
+    <row r="747" x14ac:dyDescent="0.2"/>
+    <row r="748" x14ac:dyDescent="0.2"/>
+    <row r="749" x14ac:dyDescent="0.2"/>
+    <row r="750" x14ac:dyDescent="0.2"/>
+    <row r="751" x14ac:dyDescent="0.2"/>
+    <row r="752" x14ac:dyDescent="0.2"/>
+    <row r="753" x14ac:dyDescent="0.2"/>
+    <row r="754" x14ac:dyDescent="0.2"/>
+    <row r="755" x14ac:dyDescent="0.2"/>
+    <row r="756" x14ac:dyDescent="0.2"/>
+    <row r="757" x14ac:dyDescent="0.2"/>
+    <row r="758" x14ac:dyDescent="0.2"/>
+    <row r="759" x14ac:dyDescent="0.2"/>
+    <row r="760" x14ac:dyDescent="0.2"/>
+    <row r="761" x14ac:dyDescent="0.2"/>
+    <row r="762" x14ac:dyDescent="0.2"/>
+    <row r="763" x14ac:dyDescent="0.2"/>
+    <row r="764" x14ac:dyDescent="0.2"/>
+    <row r="765" x14ac:dyDescent="0.2"/>
+    <row r="766" x14ac:dyDescent="0.2"/>
+    <row r="767" x14ac:dyDescent="0.2"/>
+    <row r="768" x14ac:dyDescent="0.2"/>
+    <row r="769" x14ac:dyDescent="0.2"/>
+    <row r="770" x14ac:dyDescent="0.2"/>
+    <row r="771" x14ac:dyDescent="0.2"/>
+    <row r="772" x14ac:dyDescent="0.2"/>
+    <row r="773" x14ac:dyDescent="0.2"/>
+    <row r="774" x14ac:dyDescent="0.2"/>
+    <row r="775" x14ac:dyDescent="0.2"/>
+    <row r="776" x14ac:dyDescent="0.2"/>
+    <row r="777" x14ac:dyDescent="0.2"/>
+    <row r="778" x14ac:dyDescent="0.2"/>
+    <row r="779" x14ac:dyDescent="0.2"/>
+    <row r="780" x14ac:dyDescent="0.2"/>
+    <row r="781" x14ac:dyDescent="0.2"/>
+    <row r="782" x14ac:dyDescent="0.2"/>
+    <row r="783" x14ac:dyDescent="0.2"/>
+    <row r="784" x14ac:dyDescent="0.2"/>
+    <row r="785" x14ac:dyDescent="0.2"/>
+    <row r="786" x14ac:dyDescent="0.2"/>
+    <row r="787" x14ac:dyDescent="0.2"/>
+    <row r="788" x14ac:dyDescent="0.2"/>
+    <row r="789" x14ac:dyDescent="0.2"/>
+    <row r="790" x14ac:dyDescent="0.2"/>
+    <row r="791" x14ac:dyDescent="0.2"/>
+    <row r="792" x14ac:dyDescent="0.2"/>
+    <row r="793" x14ac:dyDescent="0.2"/>
+    <row r="794" x14ac:dyDescent="0.2"/>
+    <row r="795" x14ac:dyDescent="0.2"/>
+    <row r="796" x14ac:dyDescent="0.2"/>
+    <row r="797" x14ac:dyDescent="0.2"/>
+    <row r="798" x14ac:dyDescent="0.2"/>
+    <row r="799" x14ac:dyDescent="0.2"/>
+    <row r="800" x14ac:dyDescent="0.2"/>
+    <row r="801" x14ac:dyDescent="0.2"/>
+    <row r="802" x14ac:dyDescent="0.2"/>
+    <row r="803" x14ac:dyDescent="0.2"/>
+    <row r="804" x14ac:dyDescent="0.2"/>
+    <row r="805" x14ac:dyDescent="0.2"/>
+    <row r="806" x14ac:dyDescent="0.2"/>
+    <row r="807" x14ac:dyDescent="0.2"/>
+    <row r="808" x14ac:dyDescent="0.2"/>
+    <row r="809" x14ac:dyDescent="0.2"/>
+    <row r="810" x14ac:dyDescent="0.2"/>
+    <row r="811" x14ac:dyDescent="0.2"/>
+    <row r="812" x14ac:dyDescent="0.2"/>
+    <row r="813" x14ac:dyDescent="0.2"/>
+    <row r="814" x14ac:dyDescent="0.2"/>
+    <row r="815" x14ac:dyDescent="0.2"/>
+    <row r="816" x14ac:dyDescent="0.2"/>
+    <row r="817" x14ac:dyDescent="0.2"/>
+    <row r="818" x14ac:dyDescent="0.2"/>
+    <row r="819" x14ac:dyDescent="0.2"/>
+    <row r="820" x14ac:dyDescent="0.2"/>
+    <row r="821" x14ac:dyDescent="0.2"/>
+    <row r="822" x14ac:dyDescent="0.2"/>
+    <row r="823" x14ac:dyDescent="0.2"/>
+    <row r="824" x14ac:dyDescent="0.2"/>
+    <row r="825" x14ac:dyDescent="0.2"/>
+    <row r="826" x14ac:dyDescent="0.2"/>
+    <row r="827" x14ac:dyDescent="0.2"/>
+    <row r="828" x14ac:dyDescent="0.2"/>
+    <row r="829" x14ac:dyDescent="0.2"/>
+    <row r="830" x14ac:dyDescent="0.2"/>
+    <row r="831" x14ac:dyDescent="0.2"/>
+    <row r="832" x14ac:dyDescent="0.2"/>
+    <row r="833" x14ac:dyDescent="0.2"/>
+    <row r="834" x14ac:dyDescent="0.2"/>
+    <row r="835" x14ac:dyDescent="0.2"/>
+    <row r="836" x14ac:dyDescent="0.2"/>
+    <row r="837" x14ac:dyDescent="0.2"/>
+    <row r="838" x14ac:dyDescent="0.2"/>
+    <row r="839" x14ac:dyDescent="0.2"/>
+    <row r="840" x14ac:dyDescent="0.2"/>
+    <row r="841" x14ac:dyDescent="0.2"/>
+    <row r="842" x14ac:dyDescent="0.2"/>
+    <row r="843" x14ac:dyDescent="0.2"/>
+    <row r="844" x14ac:dyDescent="0.2"/>
+    <row r="845" x14ac:dyDescent="0.2"/>
+    <row r="846" x14ac:dyDescent="0.2"/>
+    <row r="847" x14ac:dyDescent="0.2"/>
+    <row r="848" x14ac:dyDescent="0.2"/>
+    <row r="849" x14ac:dyDescent="0.2"/>
+    <row r="850" x14ac:dyDescent="0.2"/>
+    <row r="851" x14ac:dyDescent="0.2"/>
+    <row r="852" x14ac:dyDescent="0.2"/>
+    <row r="853" x14ac:dyDescent="0.2"/>
+    <row r="854" x14ac:dyDescent="0.2"/>
+    <row r="855" x14ac:dyDescent="0.2"/>
+    <row r="856" x14ac:dyDescent="0.2"/>
+    <row r="857" x14ac:dyDescent="0.2"/>
+    <row r="858" x14ac:dyDescent="0.2"/>
+    <row r="859" x14ac:dyDescent="0.2"/>
+    <row r="860" x14ac:dyDescent="0.2"/>
+    <row r="861" x14ac:dyDescent="0.2"/>
+    <row r="862" x14ac:dyDescent="0.2"/>
+    <row r="863" x14ac:dyDescent="0.2"/>
+    <row r="864" x14ac:dyDescent="0.2"/>
+    <row r="865" x14ac:dyDescent="0.2"/>
+    <row r="866" x14ac:dyDescent="0.2"/>
+    <row r="867" x14ac:dyDescent="0.2"/>
+    <row r="868" x14ac:dyDescent="0.2"/>
+    <row r="869" x14ac:dyDescent="0.2"/>
+    <row r="870" x14ac:dyDescent="0.2"/>
+    <row r="871" x14ac:dyDescent="0.2"/>
+    <row r="872" x14ac:dyDescent="0.2"/>
+    <row r="873" x14ac:dyDescent="0.2"/>
+    <row r="874" x14ac:dyDescent="0.2"/>
+    <row r="875" x14ac:dyDescent="0.2"/>
+    <row r="876" x14ac:dyDescent="0.2"/>
+    <row r="877" x14ac:dyDescent="0.2"/>
+    <row r="878" x14ac:dyDescent="0.2"/>
+    <row r="879" x14ac:dyDescent="0.2"/>
+    <row r="880" x14ac:dyDescent="0.2"/>
+    <row r="881" x14ac:dyDescent="0.2"/>
+    <row r="882" x14ac:dyDescent="0.2"/>
+    <row r="883" x14ac:dyDescent="0.2"/>
+    <row r="884" x14ac:dyDescent="0.2"/>
+    <row r="885" x14ac:dyDescent="0.2"/>
+    <row r="886" x14ac:dyDescent="0.2"/>
+    <row r="887" x14ac:dyDescent="0.2"/>
+    <row r="888" x14ac:dyDescent="0.2"/>
+    <row r="889" x14ac:dyDescent="0.2"/>
+    <row r="890" x14ac:dyDescent="0.2"/>
+    <row r="891" x14ac:dyDescent="0.2"/>
+    <row r="892" x14ac:dyDescent="0.2"/>
+    <row r="893" x14ac:dyDescent="0.2"/>
+    <row r="894" x14ac:dyDescent="0.2"/>
+    <row r="895" x14ac:dyDescent="0.2"/>
+    <row r="896" x14ac:dyDescent="0.2"/>
+    <row r="897" x14ac:dyDescent="0.2"/>
+    <row r="898" x14ac:dyDescent="0.2"/>
+    <row r="899" x14ac:dyDescent="0.2"/>
+    <row r="900" x14ac:dyDescent="0.2"/>
+    <row r="901" x14ac:dyDescent="0.2"/>
+    <row r="902" x14ac:dyDescent="0.2"/>
+    <row r="903" x14ac:dyDescent="0.2"/>
+    <row r="904" x14ac:dyDescent="0.2"/>
+    <row r="905" x14ac:dyDescent="0.2"/>
+    <row r="906" x14ac:dyDescent="0.2"/>
+    <row r="907" x14ac:dyDescent="0.2"/>
+    <row r="908" x14ac:dyDescent="0.2"/>
+    <row r="909" x14ac:dyDescent="0.2"/>
+    <row r="910" x14ac:dyDescent="0.2"/>
+    <row r="911" x14ac:dyDescent="0.2"/>
+    <row r="912" x14ac:dyDescent="0.2"/>
+    <row r="913" x14ac:dyDescent="0.2"/>
+    <row r="914" x14ac:dyDescent="0.2"/>
+    <row r="915" x14ac:dyDescent="0.2"/>
+    <row r="916" x14ac:dyDescent="0.2"/>
+    <row r="917" x14ac:dyDescent="0.2"/>
+    <row r="918" x14ac:dyDescent="0.2"/>
+    <row r="919" x14ac:dyDescent="0.2"/>
+    <row r="920" x14ac:dyDescent="0.2"/>
+    <row r="921" x14ac:dyDescent="0.2"/>
+    <row r="922" x14ac:dyDescent="0.2"/>
+    <row r="923" x14ac:dyDescent="0.2"/>
+    <row r="924" x14ac:dyDescent="0.2"/>
+    <row r="925" x14ac:dyDescent="0.2"/>
+    <row r="926" x14ac:dyDescent="0.2"/>
+    <row r="927" x14ac:dyDescent="0.2"/>
+    <row r="928" x14ac:dyDescent="0.2"/>
+    <row r="929" x14ac:dyDescent="0.2"/>
+    <row r="930" x14ac:dyDescent="0.2"/>
+    <row r="931" x14ac:dyDescent="0.2"/>
+    <row r="932" x14ac:dyDescent="0.2"/>
+    <row r="933" x14ac:dyDescent="0.2"/>
+    <row r="934" x14ac:dyDescent="0.2"/>
+    <row r="935" x14ac:dyDescent="0.2"/>
+    <row r="936" x14ac:dyDescent="0.2"/>
+    <row r="937" x14ac:dyDescent="0.2"/>
+    <row r="938" x14ac:dyDescent="0.2"/>
+    <row r="939" x14ac:dyDescent="0.2"/>
+    <row r="940" x14ac:dyDescent="0.2"/>
+    <row r="941" x14ac:dyDescent="0.2"/>
+    <row r="942" x14ac:dyDescent="0.2"/>
+    <row r="943" x14ac:dyDescent="0.2"/>
+    <row r="944" x14ac:dyDescent="0.2"/>
+    <row r="945" x14ac:dyDescent="0.2"/>
+    <row r="946" x14ac:dyDescent="0.2"/>
+    <row r="947" x14ac:dyDescent="0.2"/>
+    <row r="948" x14ac:dyDescent="0.2"/>
+    <row r="949" x14ac:dyDescent="0.2"/>
+    <row r="950" x14ac:dyDescent="0.2"/>
+    <row r="951" x14ac:dyDescent="0.2"/>
+    <row r="952" x14ac:dyDescent="0.2"/>
+    <row r="953" x14ac:dyDescent="0.2"/>
+    <row r="954" x14ac:dyDescent="0.2"/>
+    <row r="955" x14ac:dyDescent="0.2"/>
+    <row r="956" x14ac:dyDescent="0.2"/>
+    <row r="957" x14ac:dyDescent="0.2"/>
+    <row r="958" x14ac:dyDescent="0.2"/>
+    <row r="959" x14ac:dyDescent="0.2"/>
+    <row r="960" x14ac:dyDescent="0.2"/>
+    <row r="961" x14ac:dyDescent="0.2"/>
+    <row r="962" x14ac:dyDescent="0.2"/>
+    <row r="963" x14ac:dyDescent="0.2"/>
+    <row r="964" x14ac:dyDescent="0.2"/>
+    <row r="965" x14ac:dyDescent="0.2"/>
+    <row r="966" x14ac:dyDescent="0.2"/>
+    <row r="967" x14ac:dyDescent="0.2"/>
+    <row r="968" x14ac:dyDescent="0.2"/>
+    <row r="969" x14ac:dyDescent="0.2"/>
+    <row r="970" x14ac:dyDescent="0.2"/>
+    <row r="971" x14ac:dyDescent="0.2"/>
+    <row r="972" x14ac:dyDescent="0.2"/>
+    <row r="973" x14ac:dyDescent="0.2"/>
+    <row r="974" x14ac:dyDescent="0.2"/>
+    <row r="975" x14ac:dyDescent="0.2"/>
+    <row r="976" x14ac:dyDescent="0.2"/>
+    <row r="977" x14ac:dyDescent="0.2"/>
+    <row r="978" x14ac:dyDescent="0.2"/>
+    <row r="979" x14ac:dyDescent="0.2"/>
+    <row r="980" x14ac:dyDescent="0.2"/>
+    <row r="981" x14ac:dyDescent="0.2"/>
+    <row r="982" x14ac:dyDescent="0.2"/>
+    <row r="983" x14ac:dyDescent="0.2"/>
+    <row r="984" x14ac:dyDescent="0.2"/>
+    <row r="985" x14ac:dyDescent="0.2"/>
+    <row r="986" x14ac:dyDescent="0.2"/>
+    <row r="987" x14ac:dyDescent="0.2"/>
+    <row r="988" x14ac:dyDescent="0.2"/>
+    <row r="989" x14ac:dyDescent="0.2"/>
+    <row r="990" x14ac:dyDescent="0.2"/>
+    <row r="991" x14ac:dyDescent="0.2"/>
+    <row r="992" x14ac:dyDescent="0.2"/>
+    <row r="993" x14ac:dyDescent="0.2"/>
+    <row r="994" x14ac:dyDescent="0.2"/>
+    <row r="995" x14ac:dyDescent="0.2"/>
+    <row r="996" x14ac:dyDescent="0.2"/>
+    <row r="997" x14ac:dyDescent="0.2"/>
+    <row r="998" x14ac:dyDescent="0.2"/>
+    <row r="999" x14ac:dyDescent="0.2"/>
+    <row r="1000" x14ac:dyDescent="0.2"/>
+    <row r="1001" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9073FECC-CB4A-44B8-BFC3-FA5FF0F1128E}">
   <dimension ref="A1:D1001"/>
   <sheetViews>
@@ -2738,7 +3827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CF3190-CD72-49D9-8ABF-8252BC435300}">
   <dimension ref="A1:G1001"/>
   <sheetViews>
@@ -4864,7 +5953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -7163,6 +8252,41 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA7C6C8-3A27-4930-B617-8E2965D31C53}">
+  <dimension ref="A1:AZ1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="52" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.85546875" style="6" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9A3847-BB32-4703-88A7-C2A8351CF096}">
   <dimension ref="A1:E1001"/>
   <sheetViews>
@@ -8203,7 +9327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AZ1"/>
   <sheetViews>
@@ -8385,7 +9509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498551E9-47B3-4C71-BF2C-5EAE753DDD6D}">
   <dimension ref="A1:S1001"/>
   <sheetViews>
@@ -9473,1084 +10597,4 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38228543-4DF3-482D-9DFD-988E8DB0F6D8}">
-  <dimension ref="A1:S1001"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="12.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" style="3" hidden="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.28515625" style="3" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
-    <row r="23" x14ac:dyDescent="0.2"/>
-    <row r="24" x14ac:dyDescent="0.2"/>
-    <row r="25" x14ac:dyDescent="0.2"/>
-    <row r="26" x14ac:dyDescent="0.2"/>
-    <row r="27" x14ac:dyDescent="0.2"/>
-    <row r="28" x14ac:dyDescent="0.2"/>
-    <row r="29" x14ac:dyDescent="0.2"/>
-    <row r="30" x14ac:dyDescent="0.2"/>
-    <row r="31" x14ac:dyDescent="0.2"/>
-    <row r="32" x14ac:dyDescent="0.2"/>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
-    <row r="39" x14ac:dyDescent="0.2"/>
-    <row r="40" x14ac:dyDescent="0.2"/>
-    <row r="41" x14ac:dyDescent="0.2"/>
-    <row r="42" x14ac:dyDescent="0.2"/>
-    <row r="43" x14ac:dyDescent="0.2"/>
-    <row r="44" x14ac:dyDescent="0.2"/>
-    <row r="45" x14ac:dyDescent="0.2"/>
-    <row r="46" x14ac:dyDescent="0.2"/>
-    <row r="47" x14ac:dyDescent="0.2"/>
-    <row r="48" x14ac:dyDescent="0.2"/>
-    <row r="49" x14ac:dyDescent="0.2"/>
-    <row r="50" x14ac:dyDescent="0.2"/>
-    <row r="51" x14ac:dyDescent="0.2"/>
-    <row r="52" x14ac:dyDescent="0.2"/>
-    <row r="53" x14ac:dyDescent="0.2"/>
-    <row r="54" x14ac:dyDescent="0.2"/>
-    <row r="55" x14ac:dyDescent="0.2"/>
-    <row r="56" x14ac:dyDescent="0.2"/>
-    <row r="57" x14ac:dyDescent="0.2"/>
-    <row r="58" x14ac:dyDescent="0.2"/>
-    <row r="59" x14ac:dyDescent="0.2"/>
-    <row r="60" x14ac:dyDescent="0.2"/>
-    <row r="61" x14ac:dyDescent="0.2"/>
-    <row r="62" x14ac:dyDescent="0.2"/>
-    <row r="63" x14ac:dyDescent="0.2"/>
-    <row r="64" x14ac:dyDescent="0.2"/>
-    <row r="65" x14ac:dyDescent="0.2"/>
-    <row r="66" x14ac:dyDescent="0.2"/>
-    <row r="67" x14ac:dyDescent="0.2"/>
-    <row r="68" x14ac:dyDescent="0.2"/>
-    <row r="69" x14ac:dyDescent="0.2"/>
-    <row r="70" x14ac:dyDescent="0.2"/>
-    <row r="71" x14ac:dyDescent="0.2"/>
-    <row r="72" x14ac:dyDescent="0.2"/>
-    <row r="73" x14ac:dyDescent="0.2"/>
-    <row r="74" x14ac:dyDescent="0.2"/>
-    <row r="75" x14ac:dyDescent="0.2"/>
-    <row r="76" x14ac:dyDescent="0.2"/>
-    <row r="77" x14ac:dyDescent="0.2"/>
-    <row r="78" x14ac:dyDescent="0.2"/>
-    <row r="79" x14ac:dyDescent="0.2"/>
-    <row r="80" x14ac:dyDescent="0.2"/>
-    <row r="81" x14ac:dyDescent="0.2"/>
-    <row r="82" x14ac:dyDescent="0.2"/>
-    <row r="83" x14ac:dyDescent="0.2"/>
-    <row r="84" x14ac:dyDescent="0.2"/>
-    <row r="85" x14ac:dyDescent="0.2"/>
-    <row r="86" x14ac:dyDescent="0.2"/>
-    <row r="87" x14ac:dyDescent="0.2"/>
-    <row r="88" x14ac:dyDescent="0.2"/>
-    <row r="89" x14ac:dyDescent="0.2"/>
-    <row r="90" x14ac:dyDescent="0.2"/>
-    <row r="91" x14ac:dyDescent="0.2"/>
-    <row r="92" x14ac:dyDescent="0.2"/>
-    <row r="93" x14ac:dyDescent="0.2"/>
-    <row r="94" x14ac:dyDescent="0.2"/>
-    <row r="95" x14ac:dyDescent="0.2"/>
-    <row r="96" x14ac:dyDescent="0.2"/>
-    <row r="97" x14ac:dyDescent="0.2"/>
-    <row r="98" x14ac:dyDescent="0.2"/>
-    <row r="99" x14ac:dyDescent="0.2"/>
-    <row r="100" x14ac:dyDescent="0.2"/>
-    <row r="101" x14ac:dyDescent="0.2"/>
-    <row r="102" x14ac:dyDescent="0.2"/>
-    <row r="103" x14ac:dyDescent="0.2"/>
-    <row r="104" x14ac:dyDescent="0.2"/>
-    <row r="105" x14ac:dyDescent="0.2"/>
-    <row r="106" x14ac:dyDescent="0.2"/>
-    <row r="107" x14ac:dyDescent="0.2"/>
-    <row r="108" x14ac:dyDescent="0.2"/>
-    <row r="109" x14ac:dyDescent="0.2"/>
-    <row r="110" x14ac:dyDescent="0.2"/>
-    <row r="111" x14ac:dyDescent="0.2"/>
-    <row r="112" x14ac:dyDescent="0.2"/>
-    <row r="113" x14ac:dyDescent="0.2"/>
-    <row r="114" x14ac:dyDescent="0.2"/>
-    <row r="115" x14ac:dyDescent="0.2"/>
-    <row r="116" x14ac:dyDescent="0.2"/>
-    <row r="117" x14ac:dyDescent="0.2"/>
-    <row r="118" x14ac:dyDescent="0.2"/>
-    <row r="119" x14ac:dyDescent="0.2"/>
-    <row r="120" x14ac:dyDescent="0.2"/>
-    <row r="121" x14ac:dyDescent="0.2"/>
-    <row r="122" x14ac:dyDescent="0.2"/>
-    <row r="123" x14ac:dyDescent="0.2"/>
-    <row r="124" x14ac:dyDescent="0.2"/>
-    <row r="125" x14ac:dyDescent="0.2"/>
-    <row r="126" x14ac:dyDescent="0.2"/>
-    <row r="127" x14ac:dyDescent="0.2"/>
-    <row r="128" x14ac:dyDescent="0.2"/>
-    <row r="129" x14ac:dyDescent="0.2"/>
-    <row r="130" x14ac:dyDescent="0.2"/>
-    <row r="131" x14ac:dyDescent="0.2"/>
-    <row r="132" x14ac:dyDescent="0.2"/>
-    <row r="133" x14ac:dyDescent="0.2"/>
-    <row r="134" x14ac:dyDescent="0.2"/>
-    <row r="135" x14ac:dyDescent="0.2"/>
-    <row r="136" x14ac:dyDescent="0.2"/>
-    <row r="137" x14ac:dyDescent="0.2"/>
-    <row r="138" x14ac:dyDescent="0.2"/>
-    <row r="139" x14ac:dyDescent="0.2"/>
-    <row r="140" x14ac:dyDescent="0.2"/>
-    <row r="141" x14ac:dyDescent="0.2"/>
-    <row r="142" x14ac:dyDescent="0.2"/>
-    <row r="143" x14ac:dyDescent="0.2"/>
-    <row r="144" x14ac:dyDescent="0.2"/>
-    <row r="145" x14ac:dyDescent="0.2"/>
-    <row r="146" x14ac:dyDescent="0.2"/>
-    <row r="147" x14ac:dyDescent="0.2"/>
-    <row r="148" x14ac:dyDescent="0.2"/>
-    <row r="149" x14ac:dyDescent="0.2"/>
-    <row r="150" x14ac:dyDescent="0.2"/>
-    <row r="151" x14ac:dyDescent="0.2"/>
-    <row r="152" x14ac:dyDescent="0.2"/>
-    <row r="153" x14ac:dyDescent="0.2"/>
-    <row r="154" x14ac:dyDescent="0.2"/>
-    <row r="155" x14ac:dyDescent="0.2"/>
-    <row r="156" x14ac:dyDescent="0.2"/>
-    <row r="157" x14ac:dyDescent="0.2"/>
-    <row r="158" x14ac:dyDescent="0.2"/>
-    <row r="159" x14ac:dyDescent="0.2"/>
-    <row r="160" x14ac:dyDescent="0.2"/>
-    <row r="161" x14ac:dyDescent="0.2"/>
-    <row r="162" x14ac:dyDescent="0.2"/>
-    <row r="163" x14ac:dyDescent="0.2"/>
-    <row r="164" x14ac:dyDescent="0.2"/>
-    <row r="165" x14ac:dyDescent="0.2"/>
-    <row r="166" x14ac:dyDescent="0.2"/>
-    <row r="167" x14ac:dyDescent="0.2"/>
-    <row r="168" x14ac:dyDescent="0.2"/>
-    <row r="169" x14ac:dyDescent="0.2"/>
-    <row r="170" x14ac:dyDescent="0.2"/>
-    <row r="171" x14ac:dyDescent="0.2"/>
-    <row r="172" x14ac:dyDescent="0.2"/>
-    <row r="173" x14ac:dyDescent="0.2"/>
-    <row r="174" x14ac:dyDescent="0.2"/>
-    <row r="175" x14ac:dyDescent="0.2"/>
-    <row r="176" x14ac:dyDescent="0.2"/>
-    <row r="177" x14ac:dyDescent="0.2"/>
-    <row r="178" x14ac:dyDescent="0.2"/>
-    <row r="179" x14ac:dyDescent="0.2"/>
-    <row r="180" x14ac:dyDescent="0.2"/>
-    <row r="181" x14ac:dyDescent="0.2"/>
-    <row r="182" x14ac:dyDescent="0.2"/>
-    <row r="183" x14ac:dyDescent="0.2"/>
-    <row r="184" x14ac:dyDescent="0.2"/>
-    <row r="185" x14ac:dyDescent="0.2"/>
-    <row r="186" x14ac:dyDescent="0.2"/>
-    <row r="187" x14ac:dyDescent="0.2"/>
-    <row r="188" x14ac:dyDescent="0.2"/>
-    <row r="189" x14ac:dyDescent="0.2"/>
-    <row r="190" x14ac:dyDescent="0.2"/>
-    <row r="191" x14ac:dyDescent="0.2"/>
-    <row r="192" x14ac:dyDescent="0.2"/>
-    <row r="193" x14ac:dyDescent="0.2"/>
-    <row r="194" x14ac:dyDescent="0.2"/>
-    <row r="195" x14ac:dyDescent="0.2"/>
-    <row r="196" x14ac:dyDescent="0.2"/>
-    <row r="197" x14ac:dyDescent="0.2"/>
-    <row r="198" x14ac:dyDescent="0.2"/>
-    <row r="199" x14ac:dyDescent="0.2"/>
-    <row r="200" x14ac:dyDescent="0.2"/>
-    <row r="201" x14ac:dyDescent="0.2"/>
-    <row r="202" x14ac:dyDescent="0.2"/>
-    <row r="203" x14ac:dyDescent="0.2"/>
-    <row r="204" x14ac:dyDescent="0.2"/>
-    <row r="205" x14ac:dyDescent="0.2"/>
-    <row r="206" x14ac:dyDescent="0.2"/>
-    <row r="207" x14ac:dyDescent="0.2"/>
-    <row r="208" x14ac:dyDescent="0.2"/>
-    <row r="209" x14ac:dyDescent="0.2"/>
-    <row r="210" x14ac:dyDescent="0.2"/>
-    <row r="211" x14ac:dyDescent="0.2"/>
-    <row r="212" x14ac:dyDescent="0.2"/>
-    <row r="213" x14ac:dyDescent="0.2"/>
-    <row r="214" x14ac:dyDescent="0.2"/>
-    <row r="215" x14ac:dyDescent="0.2"/>
-    <row r="216" x14ac:dyDescent="0.2"/>
-    <row r="217" x14ac:dyDescent="0.2"/>
-    <row r="218" x14ac:dyDescent="0.2"/>
-    <row r="219" x14ac:dyDescent="0.2"/>
-    <row r="220" x14ac:dyDescent="0.2"/>
-    <row r="221" x14ac:dyDescent="0.2"/>
-    <row r="222" x14ac:dyDescent="0.2"/>
-    <row r="223" x14ac:dyDescent="0.2"/>
-    <row r="224" x14ac:dyDescent="0.2"/>
-    <row r="225" x14ac:dyDescent="0.2"/>
-    <row r="226" x14ac:dyDescent="0.2"/>
-    <row r="227" x14ac:dyDescent="0.2"/>
-    <row r="228" x14ac:dyDescent="0.2"/>
-    <row r="229" x14ac:dyDescent="0.2"/>
-    <row r="230" x14ac:dyDescent="0.2"/>
-    <row r="231" x14ac:dyDescent="0.2"/>
-    <row r="232" x14ac:dyDescent="0.2"/>
-    <row r="233" x14ac:dyDescent="0.2"/>
-    <row r="234" x14ac:dyDescent="0.2"/>
-    <row r="235" x14ac:dyDescent="0.2"/>
-    <row r="236" x14ac:dyDescent="0.2"/>
-    <row r="237" x14ac:dyDescent="0.2"/>
-    <row r="238" x14ac:dyDescent="0.2"/>
-    <row r="239" x14ac:dyDescent="0.2"/>
-    <row r="240" x14ac:dyDescent="0.2"/>
-    <row r="241" x14ac:dyDescent="0.2"/>
-    <row r="242" x14ac:dyDescent="0.2"/>
-    <row r="243" x14ac:dyDescent="0.2"/>
-    <row r="244" x14ac:dyDescent="0.2"/>
-    <row r="245" x14ac:dyDescent="0.2"/>
-    <row r="246" x14ac:dyDescent="0.2"/>
-    <row r="247" x14ac:dyDescent="0.2"/>
-    <row r="248" x14ac:dyDescent="0.2"/>
-    <row r="249" x14ac:dyDescent="0.2"/>
-    <row r="250" x14ac:dyDescent="0.2"/>
-    <row r="251" x14ac:dyDescent="0.2"/>
-    <row r="252" x14ac:dyDescent="0.2"/>
-    <row r="253" x14ac:dyDescent="0.2"/>
-    <row r="254" x14ac:dyDescent="0.2"/>
-    <row r="255" x14ac:dyDescent="0.2"/>
-    <row r="256" x14ac:dyDescent="0.2"/>
-    <row r="257" x14ac:dyDescent="0.2"/>
-    <row r="258" x14ac:dyDescent="0.2"/>
-    <row r="259" x14ac:dyDescent="0.2"/>
-    <row r="260" x14ac:dyDescent="0.2"/>
-    <row r="261" x14ac:dyDescent="0.2"/>
-    <row r="262" x14ac:dyDescent="0.2"/>
-    <row r="263" x14ac:dyDescent="0.2"/>
-    <row r="264" x14ac:dyDescent="0.2"/>
-    <row r="265" x14ac:dyDescent="0.2"/>
-    <row r="266" x14ac:dyDescent="0.2"/>
-    <row r="267" x14ac:dyDescent="0.2"/>
-    <row r="268" x14ac:dyDescent="0.2"/>
-    <row r="269" x14ac:dyDescent="0.2"/>
-    <row r="270" x14ac:dyDescent="0.2"/>
-    <row r="271" x14ac:dyDescent="0.2"/>
-    <row r="272" x14ac:dyDescent="0.2"/>
-    <row r="273" x14ac:dyDescent="0.2"/>
-    <row r="274" x14ac:dyDescent="0.2"/>
-    <row r="275" x14ac:dyDescent="0.2"/>
-    <row r="276" x14ac:dyDescent="0.2"/>
-    <row r="277" x14ac:dyDescent="0.2"/>
-    <row r="278" x14ac:dyDescent="0.2"/>
-    <row r="279" x14ac:dyDescent="0.2"/>
-    <row r="280" x14ac:dyDescent="0.2"/>
-    <row r="281" x14ac:dyDescent="0.2"/>
-    <row r="282" x14ac:dyDescent="0.2"/>
-    <row r="283" x14ac:dyDescent="0.2"/>
-    <row r="284" x14ac:dyDescent="0.2"/>
-    <row r="285" x14ac:dyDescent="0.2"/>
-    <row r="286" x14ac:dyDescent="0.2"/>
-    <row r="287" x14ac:dyDescent="0.2"/>
-    <row r="288" x14ac:dyDescent="0.2"/>
-    <row r="289" x14ac:dyDescent="0.2"/>
-    <row r="290" x14ac:dyDescent="0.2"/>
-    <row r="291" x14ac:dyDescent="0.2"/>
-    <row r="292" x14ac:dyDescent="0.2"/>
-    <row r="293" x14ac:dyDescent="0.2"/>
-    <row r="294" x14ac:dyDescent="0.2"/>
-    <row r="295" x14ac:dyDescent="0.2"/>
-    <row r="296" x14ac:dyDescent="0.2"/>
-    <row r="297" x14ac:dyDescent="0.2"/>
-    <row r="298" x14ac:dyDescent="0.2"/>
-    <row r="299" x14ac:dyDescent="0.2"/>
-    <row r="300" x14ac:dyDescent="0.2"/>
-    <row r="301" x14ac:dyDescent="0.2"/>
-    <row r="302" x14ac:dyDescent="0.2"/>
-    <row r="303" x14ac:dyDescent="0.2"/>
-    <row r="304" x14ac:dyDescent="0.2"/>
-    <row r="305" x14ac:dyDescent="0.2"/>
-    <row r="306" x14ac:dyDescent="0.2"/>
-    <row r="307" x14ac:dyDescent="0.2"/>
-    <row r="308" x14ac:dyDescent="0.2"/>
-    <row r="309" x14ac:dyDescent="0.2"/>
-    <row r="310" x14ac:dyDescent="0.2"/>
-    <row r="311" x14ac:dyDescent="0.2"/>
-    <row r="312" x14ac:dyDescent="0.2"/>
-    <row r="313" x14ac:dyDescent="0.2"/>
-    <row r="314" x14ac:dyDescent="0.2"/>
-    <row r="315" x14ac:dyDescent="0.2"/>
-    <row r="316" x14ac:dyDescent="0.2"/>
-    <row r="317" x14ac:dyDescent="0.2"/>
-    <row r="318" x14ac:dyDescent="0.2"/>
-    <row r="319" x14ac:dyDescent="0.2"/>
-    <row r="320" x14ac:dyDescent="0.2"/>
-    <row r="321" x14ac:dyDescent="0.2"/>
-    <row r="322" x14ac:dyDescent="0.2"/>
-    <row r="323" x14ac:dyDescent="0.2"/>
-    <row r="324" x14ac:dyDescent="0.2"/>
-    <row r="325" x14ac:dyDescent="0.2"/>
-    <row r="326" x14ac:dyDescent="0.2"/>
-    <row r="327" x14ac:dyDescent="0.2"/>
-    <row r="328" x14ac:dyDescent="0.2"/>
-    <row r="329" x14ac:dyDescent="0.2"/>
-    <row r="330" x14ac:dyDescent="0.2"/>
-    <row r="331" x14ac:dyDescent="0.2"/>
-    <row r="332" x14ac:dyDescent="0.2"/>
-    <row r="333" x14ac:dyDescent="0.2"/>
-    <row r="334" x14ac:dyDescent="0.2"/>
-    <row r="335" x14ac:dyDescent="0.2"/>
-    <row r="336" x14ac:dyDescent="0.2"/>
-    <row r="337" x14ac:dyDescent="0.2"/>
-    <row r="338" x14ac:dyDescent="0.2"/>
-    <row r="339" x14ac:dyDescent="0.2"/>
-    <row r="340" x14ac:dyDescent="0.2"/>
-    <row r="341" x14ac:dyDescent="0.2"/>
-    <row r="342" x14ac:dyDescent="0.2"/>
-    <row r="343" x14ac:dyDescent="0.2"/>
-    <row r="344" x14ac:dyDescent="0.2"/>
-    <row r="345" x14ac:dyDescent="0.2"/>
-    <row r="346" x14ac:dyDescent="0.2"/>
-    <row r="347" x14ac:dyDescent="0.2"/>
-    <row r="348" x14ac:dyDescent="0.2"/>
-    <row r="349" x14ac:dyDescent="0.2"/>
-    <row r="350" x14ac:dyDescent="0.2"/>
-    <row r="351" x14ac:dyDescent="0.2"/>
-    <row r="352" x14ac:dyDescent="0.2"/>
-    <row r="353" x14ac:dyDescent="0.2"/>
-    <row r="354" x14ac:dyDescent="0.2"/>
-    <row r="355" x14ac:dyDescent="0.2"/>
-    <row r="356" x14ac:dyDescent="0.2"/>
-    <row r="357" x14ac:dyDescent="0.2"/>
-    <row r="358" x14ac:dyDescent="0.2"/>
-    <row r="359" x14ac:dyDescent="0.2"/>
-    <row r="360" x14ac:dyDescent="0.2"/>
-    <row r="361" x14ac:dyDescent="0.2"/>
-    <row r="362" x14ac:dyDescent="0.2"/>
-    <row r="363" x14ac:dyDescent="0.2"/>
-    <row r="364" x14ac:dyDescent="0.2"/>
-    <row r="365" x14ac:dyDescent="0.2"/>
-    <row r="366" x14ac:dyDescent="0.2"/>
-    <row r="367" x14ac:dyDescent="0.2"/>
-    <row r="368" x14ac:dyDescent="0.2"/>
-    <row r="369" x14ac:dyDescent="0.2"/>
-    <row r="370" x14ac:dyDescent="0.2"/>
-    <row r="371" x14ac:dyDescent="0.2"/>
-    <row r="372" x14ac:dyDescent="0.2"/>
-    <row r="373" x14ac:dyDescent="0.2"/>
-    <row r="374" x14ac:dyDescent="0.2"/>
-    <row r="375" x14ac:dyDescent="0.2"/>
-    <row r="376" x14ac:dyDescent="0.2"/>
-    <row r="377" x14ac:dyDescent="0.2"/>
-    <row r="378" x14ac:dyDescent="0.2"/>
-    <row r="379" x14ac:dyDescent="0.2"/>
-    <row r="380" x14ac:dyDescent="0.2"/>
-    <row r="381" x14ac:dyDescent="0.2"/>
-    <row r="382" x14ac:dyDescent="0.2"/>
-    <row r="383" x14ac:dyDescent="0.2"/>
-    <row r="384" x14ac:dyDescent="0.2"/>
-    <row r="385" x14ac:dyDescent="0.2"/>
-    <row r="386" x14ac:dyDescent="0.2"/>
-    <row r="387" x14ac:dyDescent="0.2"/>
-    <row r="388" x14ac:dyDescent="0.2"/>
-    <row r="389" x14ac:dyDescent="0.2"/>
-    <row r="390" x14ac:dyDescent="0.2"/>
-    <row r="391" x14ac:dyDescent="0.2"/>
-    <row r="392" x14ac:dyDescent="0.2"/>
-    <row r="393" x14ac:dyDescent="0.2"/>
-    <row r="394" x14ac:dyDescent="0.2"/>
-    <row r="395" x14ac:dyDescent="0.2"/>
-    <row r="396" x14ac:dyDescent="0.2"/>
-    <row r="397" x14ac:dyDescent="0.2"/>
-    <row r="398" x14ac:dyDescent="0.2"/>
-    <row r="399" x14ac:dyDescent="0.2"/>
-    <row r="400" x14ac:dyDescent="0.2"/>
-    <row r="401" x14ac:dyDescent="0.2"/>
-    <row r="402" x14ac:dyDescent="0.2"/>
-    <row r="403" x14ac:dyDescent="0.2"/>
-    <row r="404" x14ac:dyDescent="0.2"/>
-    <row r="405" x14ac:dyDescent="0.2"/>
-    <row r="406" x14ac:dyDescent="0.2"/>
-    <row r="407" x14ac:dyDescent="0.2"/>
-    <row r="408" x14ac:dyDescent="0.2"/>
-    <row r="409" x14ac:dyDescent="0.2"/>
-    <row r="410" x14ac:dyDescent="0.2"/>
-    <row r="411" x14ac:dyDescent="0.2"/>
-    <row r="412" x14ac:dyDescent="0.2"/>
-    <row r="413" x14ac:dyDescent="0.2"/>
-    <row r="414" x14ac:dyDescent="0.2"/>
-    <row r="415" x14ac:dyDescent="0.2"/>
-    <row r="416" x14ac:dyDescent="0.2"/>
-    <row r="417" x14ac:dyDescent="0.2"/>
-    <row r="418" x14ac:dyDescent="0.2"/>
-    <row r="419" x14ac:dyDescent="0.2"/>
-    <row r="420" x14ac:dyDescent="0.2"/>
-    <row r="421" x14ac:dyDescent="0.2"/>
-    <row r="422" x14ac:dyDescent="0.2"/>
-    <row r="423" x14ac:dyDescent="0.2"/>
-    <row r="424" x14ac:dyDescent="0.2"/>
-    <row r="425" x14ac:dyDescent="0.2"/>
-    <row r="426" x14ac:dyDescent="0.2"/>
-    <row r="427" x14ac:dyDescent="0.2"/>
-    <row r="428" x14ac:dyDescent="0.2"/>
-    <row r="429" x14ac:dyDescent="0.2"/>
-    <row r="430" x14ac:dyDescent="0.2"/>
-    <row r="431" x14ac:dyDescent="0.2"/>
-    <row r="432" x14ac:dyDescent="0.2"/>
-    <row r="433" x14ac:dyDescent="0.2"/>
-    <row r="434" x14ac:dyDescent="0.2"/>
-    <row r="435" x14ac:dyDescent="0.2"/>
-    <row r="436" x14ac:dyDescent="0.2"/>
-    <row r="437" x14ac:dyDescent="0.2"/>
-    <row r="438" x14ac:dyDescent="0.2"/>
-    <row r="439" x14ac:dyDescent="0.2"/>
-    <row r="440" x14ac:dyDescent="0.2"/>
-    <row r="441" x14ac:dyDescent="0.2"/>
-    <row r="442" x14ac:dyDescent="0.2"/>
-    <row r="443" x14ac:dyDescent="0.2"/>
-    <row r="444" x14ac:dyDescent="0.2"/>
-    <row r="445" x14ac:dyDescent="0.2"/>
-    <row r="446" x14ac:dyDescent="0.2"/>
-    <row r="447" x14ac:dyDescent="0.2"/>
-    <row r="448" x14ac:dyDescent="0.2"/>
-    <row r="449" x14ac:dyDescent="0.2"/>
-    <row r="450" x14ac:dyDescent="0.2"/>
-    <row r="451" x14ac:dyDescent="0.2"/>
-    <row r="452" x14ac:dyDescent="0.2"/>
-    <row r="453" x14ac:dyDescent="0.2"/>
-    <row r="454" x14ac:dyDescent="0.2"/>
-    <row r="455" x14ac:dyDescent="0.2"/>
-    <row r="456" x14ac:dyDescent="0.2"/>
-    <row r="457" x14ac:dyDescent="0.2"/>
-    <row r="458" x14ac:dyDescent="0.2"/>
-    <row r="459" x14ac:dyDescent="0.2"/>
-    <row r="460" x14ac:dyDescent="0.2"/>
-    <row r="461" x14ac:dyDescent="0.2"/>
-    <row r="462" x14ac:dyDescent="0.2"/>
-    <row r="463" x14ac:dyDescent="0.2"/>
-    <row r="464" x14ac:dyDescent="0.2"/>
-    <row r="465" x14ac:dyDescent="0.2"/>
-    <row r="466" x14ac:dyDescent="0.2"/>
-    <row r="467" x14ac:dyDescent="0.2"/>
-    <row r="468" x14ac:dyDescent="0.2"/>
-    <row r="469" x14ac:dyDescent="0.2"/>
-    <row r="470" x14ac:dyDescent="0.2"/>
-    <row r="471" x14ac:dyDescent="0.2"/>
-    <row r="472" x14ac:dyDescent="0.2"/>
-    <row r="473" x14ac:dyDescent="0.2"/>
-    <row r="474" x14ac:dyDescent="0.2"/>
-    <row r="475" x14ac:dyDescent="0.2"/>
-    <row r="476" x14ac:dyDescent="0.2"/>
-    <row r="477" x14ac:dyDescent="0.2"/>
-    <row r="478" x14ac:dyDescent="0.2"/>
-    <row r="479" x14ac:dyDescent="0.2"/>
-    <row r="480" x14ac:dyDescent="0.2"/>
-    <row r="481" x14ac:dyDescent="0.2"/>
-    <row r="482" x14ac:dyDescent="0.2"/>
-    <row r="483" x14ac:dyDescent="0.2"/>
-    <row r="484" x14ac:dyDescent="0.2"/>
-    <row r="485" x14ac:dyDescent="0.2"/>
-    <row r="486" x14ac:dyDescent="0.2"/>
-    <row r="487" x14ac:dyDescent="0.2"/>
-    <row r="488" x14ac:dyDescent="0.2"/>
-    <row r="489" x14ac:dyDescent="0.2"/>
-    <row r="490" x14ac:dyDescent="0.2"/>
-    <row r="491" x14ac:dyDescent="0.2"/>
-    <row r="492" x14ac:dyDescent="0.2"/>
-    <row r="493" x14ac:dyDescent="0.2"/>
-    <row r="494" x14ac:dyDescent="0.2"/>
-    <row r="495" x14ac:dyDescent="0.2"/>
-    <row r="496" x14ac:dyDescent="0.2"/>
-    <row r="497" x14ac:dyDescent="0.2"/>
-    <row r="498" x14ac:dyDescent="0.2"/>
-    <row r="499" x14ac:dyDescent="0.2"/>
-    <row r="500" x14ac:dyDescent="0.2"/>
-    <row r="501" x14ac:dyDescent="0.2"/>
-    <row r="502" x14ac:dyDescent="0.2"/>
-    <row r="503" x14ac:dyDescent="0.2"/>
-    <row r="504" x14ac:dyDescent="0.2"/>
-    <row r="505" x14ac:dyDescent="0.2"/>
-    <row r="506" x14ac:dyDescent="0.2"/>
-    <row r="507" x14ac:dyDescent="0.2"/>
-    <row r="508" x14ac:dyDescent="0.2"/>
-    <row r="509" x14ac:dyDescent="0.2"/>
-    <row r="510" x14ac:dyDescent="0.2"/>
-    <row r="511" x14ac:dyDescent="0.2"/>
-    <row r="512" x14ac:dyDescent="0.2"/>
-    <row r="513" x14ac:dyDescent="0.2"/>
-    <row r="514" x14ac:dyDescent="0.2"/>
-    <row r="515" x14ac:dyDescent="0.2"/>
-    <row r="516" x14ac:dyDescent="0.2"/>
-    <row r="517" x14ac:dyDescent="0.2"/>
-    <row r="518" x14ac:dyDescent="0.2"/>
-    <row r="519" x14ac:dyDescent="0.2"/>
-    <row r="520" x14ac:dyDescent="0.2"/>
-    <row r="521" x14ac:dyDescent="0.2"/>
-    <row r="522" x14ac:dyDescent="0.2"/>
-    <row r="523" x14ac:dyDescent="0.2"/>
-    <row r="524" x14ac:dyDescent="0.2"/>
-    <row r="525" x14ac:dyDescent="0.2"/>
-    <row r="526" x14ac:dyDescent="0.2"/>
-    <row r="527" x14ac:dyDescent="0.2"/>
-    <row r="528" x14ac:dyDescent="0.2"/>
-    <row r="529" x14ac:dyDescent="0.2"/>
-    <row r="530" x14ac:dyDescent="0.2"/>
-    <row r="531" x14ac:dyDescent="0.2"/>
-    <row r="532" x14ac:dyDescent="0.2"/>
-    <row r="533" x14ac:dyDescent="0.2"/>
-    <row r="534" x14ac:dyDescent="0.2"/>
-    <row r="535" x14ac:dyDescent="0.2"/>
-    <row r="536" x14ac:dyDescent="0.2"/>
-    <row r="537" x14ac:dyDescent="0.2"/>
-    <row r="538" x14ac:dyDescent="0.2"/>
-    <row r="539" x14ac:dyDescent="0.2"/>
-    <row r="540" x14ac:dyDescent="0.2"/>
-    <row r="541" x14ac:dyDescent="0.2"/>
-    <row r="542" x14ac:dyDescent="0.2"/>
-    <row r="543" x14ac:dyDescent="0.2"/>
-    <row r="544" x14ac:dyDescent="0.2"/>
-    <row r="545" x14ac:dyDescent="0.2"/>
-    <row r="546" x14ac:dyDescent="0.2"/>
-    <row r="547" x14ac:dyDescent="0.2"/>
-    <row r="548" x14ac:dyDescent="0.2"/>
-    <row r="549" x14ac:dyDescent="0.2"/>
-    <row r="550" x14ac:dyDescent="0.2"/>
-    <row r="551" x14ac:dyDescent="0.2"/>
-    <row r="552" x14ac:dyDescent="0.2"/>
-    <row r="553" x14ac:dyDescent="0.2"/>
-    <row r="554" x14ac:dyDescent="0.2"/>
-    <row r="555" x14ac:dyDescent="0.2"/>
-    <row r="556" x14ac:dyDescent="0.2"/>
-    <row r="557" x14ac:dyDescent="0.2"/>
-    <row r="558" x14ac:dyDescent="0.2"/>
-    <row r="559" x14ac:dyDescent="0.2"/>
-    <row r="560" x14ac:dyDescent="0.2"/>
-    <row r="561" x14ac:dyDescent="0.2"/>
-    <row r="562" x14ac:dyDescent="0.2"/>
-    <row r="563" x14ac:dyDescent="0.2"/>
-    <row r="564" x14ac:dyDescent="0.2"/>
-    <row r="565" x14ac:dyDescent="0.2"/>
-    <row r="566" x14ac:dyDescent="0.2"/>
-    <row r="567" x14ac:dyDescent="0.2"/>
-    <row r="568" x14ac:dyDescent="0.2"/>
-    <row r="569" x14ac:dyDescent="0.2"/>
-    <row r="570" x14ac:dyDescent="0.2"/>
-    <row r="571" x14ac:dyDescent="0.2"/>
-    <row r="572" x14ac:dyDescent="0.2"/>
-    <row r="573" x14ac:dyDescent="0.2"/>
-    <row r="574" x14ac:dyDescent="0.2"/>
-    <row r="575" x14ac:dyDescent="0.2"/>
-    <row r="576" x14ac:dyDescent="0.2"/>
-    <row r="577" x14ac:dyDescent="0.2"/>
-    <row r="578" x14ac:dyDescent="0.2"/>
-    <row r="579" x14ac:dyDescent="0.2"/>
-    <row r="580" x14ac:dyDescent="0.2"/>
-    <row r="581" x14ac:dyDescent="0.2"/>
-    <row r="582" x14ac:dyDescent="0.2"/>
-    <row r="583" x14ac:dyDescent="0.2"/>
-    <row r="584" x14ac:dyDescent="0.2"/>
-    <row r="585" x14ac:dyDescent="0.2"/>
-    <row r="586" x14ac:dyDescent="0.2"/>
-    <row r="587" x14ac:dyDescent="0.2"/>
-    <row r="588" x14ac:dyDescent="0.2"/>
-    <row r="589" x14ac:dyDescent="0.2"/>
-    <row r="590" x14ac:dyDescent="0.2"/>
-    <row r="591" x14ac:dyDescent="0.2"/>
-    <row r="592" x14ac:dyDescent="0.2"/>
-    <row r="593" x14ac:dyDescent="0.2"/>
-    <row r="594" x14ac:dyDescent="0.2"/>
-    <row r="595" x14ac:dyDescent="0.2"/>
-    <row r="596" x14ac:dyDescent="0.2"/>
-    <row r="597" x14ac:dyDescent="0.2"/>
-    <row r="598" x14ac:dyDescent="0.2"/>
-    <row r="599" x14ac:dyDescent="0.2"/>
-    <row r="600" x14ac:dyDescent="0.2"/>
-    <row r="601" x14ac:dyDescent="0.2"/>
-    <row r="602" x14ac:dyDescent="0.2"/>
-    <row r="603" x14ac:dyDescent="0.2"/>
-    <row r="604" x14ac:dyDescent="0.2"/>
-    <row r="605" x14ac:dyDescent="0.2"/>
-    <row r="606" x14ac:dyDescent="0.2"/>
-    <row r="607" x14ac:dyDescent="0.2"/>
-    <row r="608" x14ac:dyDescent="0.2"/>
-    <row r="609" x14ac:dyDescent="0.2"/>
-    <row r="610" x14ac:dyDescent="0.2"/>
-    <row r="611" x14ac:dyDescent="0.2"/>
-    <row r="612" x14ac:dyDescent="0.2"/>
-    <row r="613" x14ac:dyDescent="0.2"/>
-    <row r="614" x14ac:dyDescent="0.2"/>
-    <row r="615" x14ac:dyDescent="0.2"/>
-    <row r="616" x14ac:dyDescent="0.2"/>
-    <row r="617" x14ac:dyDescent="0.2"/>
-    <row r="618" x14ac:dyDescent="0.2"/>
-    <row r="619" x14ac:dyDescent="0.2"/>
-    <row r="620" x14ac:dyDescent="0.2"/>
-    <row r="621" x14ac:dyDescent="0.2"/>
-    <row r="622" x14ac:dyDescent="0.2"/>
-    <row r="623" x14ac:dyDescent="0.2"/>
-    <row r="624" x14ac:dyDescent="0.2"/>
-    <row r="625" x14ac:dyDescent="0.2"/>
-    <row r="626" x14ac:dyDescent="0.2"/>
-    <row r="627" x14ac:dyDescent="0.2"/>
-    <row r="628" x14ac:dyDescent="0.2"/>
-    <row r="629" x14ac:dyDescent="0.2"/>
-    <row r="630" x14ac:dyDescent="0.2"/>
-    <row r="631" x14ac:dyDescent="0.2"/>
-    <row r="632" x14ac:dyDescent="0.2"/>
-    <row r="633" x14ac:dyDescent="0.2"/>
-    <row r="634" x14ac:dyDescent="0.2"/>
-    <row r="635" x14ac:dyDescent="0.2"/>
-    <row r="636" x14ac:dyDescent="0.2"/>
-    <row r="637" x14ac:dyDescent="0.2"/>
-    <row r="638" x14ac:dyDescent="0.2"/>
-    <row r="639" x14ac:dyDescent="0.2"/>
-    <row r="640" x14ac:dyDescent="0.2"/>
-    <row r="641" x14ac:dyDescent="0.2"/>
-    <row r="642" x14ac:dyDescent="0.2"/>
-    <row r="643" x14ac:dyDescent="0.2"/>
-    <row r="644" x14ac:dyDescent="0.2"/>
-    <row r="645" x14ac:dyDescent="0.2"/>
-    <row r="646" x14ac:dyDescent="0.2"/>
-    <row r="647" x14ac:dyDescent="0.2"/>
-    <row r="648" x14ac:dyDescent="0.2"/>
-    <row r="649" x14ac:dyDescent="0.2"/>
-    <row r="650" x14ac:dyDescent="0.2"/>
-    <row r="651" x14ac:dyDescent="0.2"/>
-    <row r="652" x14ac:dyDescent="0.2"/>
-    <row r="653" x14ac:dyDescent="0.2"/>
-    <row r="654" x14ac:dyDescent="0.2"/>
-    <row r="655" x14ac:dyDescent="0.2"/>
-    <row r="656" x14ac:dyDescent="0.2"/>
-    <row r="657" x14ac:dyDescent="0.2"/>
-    <row r="658" x14ac:dyDescent="0.2"/>
-    <row r="659" x14ac:dyDescent="0.2"/>
-    <row r="660" x14ac:dyDescent="0.2"/>
-    <row r="661" x14ac:dyDescent="0.2"/>
-    <row r="662" x14ac:dyDescent="0.2"/>
-    <row r="663" x14ac:dyDescent="0.2"/>
-    <row r="664" x14ac:dyDescent="0.2"/>
-    <row r="665" x14ac:dyDescent="0.2"/>
-    <row r="666" x14ac:dyDescent="0.2"/>
-    <row r="667" x14ac:dyDescent="0.2"/>
-    <row r="668" x14ac:dyDescent="0.2"/>
-    <row r="669" x14ac:dyDescent="0.2"/>
-    <row r="670" x14ac:dyDescent="0.2"/>
-    <row r="671" x14ac:dyDescent="0.2"/>
-    <row r="672" x14ac:dyDescent="0.2"/>
-    <row r="673" x14ac:dyDescent="0.2"/>
-    <row r="674" x14ac:dyDescent="0.2"/>
-    <row r="675" x14ac:dyDescent="0.2"/>
-    <row r="676" x14ac:dyDescent="0.2"/>
-    <row r="677" x14ac:dyDescent="0.2"/>
-    <row r="678" x14ac:dyDescent="0.2"/>
-    <row r="679" x14ac:dyDescent="0.2"/>
-    <row r="680" x14ac:dyDescent="0.2"/>
-    <row r="681" x14ac:dyDescent="0.2"/>
-    <row r="682" x14ac:dyDescent="0.2"/>
-    <row r="683" x14ac:dyDescent="0.2"/>
-    <row r="684" x14ac:dyDescent="0.2"/>
-    <row r="685" x14ac:dyDescent="0.2"/>
-    <row r="686" x14ac:dyDescent="0.2"/>
-    <row r="687" x14ac:dyDescent="0.2"/>
-    <row r="688" x14ac:dyDescent="0.2"/>
-    <row r="689" x14ac:dyDescent="0.2"/>
-    <row r="690" x14ac:dyDescent="0.2"/>
-    <row r="691" x14ac:dyDescent="0.2"/>
-    <row r="692" x14ac:dyDescent="0.2"/>
-    <row r="693" x14ac:dyDescent="0.2"/>
-    <row r="694" x14ac:dyDescent="0.2"/>
-    <row r="695" x14ac:dyDescent="0.2"/>
-    <row r="696" x14ac:dyDescent="0.2"/>
-    <row r="697" x14ac:dyDescent="0.2"/>
-    <row r="698" x14ac:dyDescent="0.2"/>
-    <row r="699" x14ac:dyDescent="0.2"/>
-    <row r="700" x14ac:dyDescent="0.2"/>
-    <row r="701" x14ac:dyDescent="0.2"/>
-    <row r="702" x14ac:dyDescent="0.2"/>
-    <row r="703" x14ac:dyDescent="0.2"/>
-    <row r="704" x14ac:dyDescent="0.2"/>
-    <row r="705" x14ac:dyDescent="0.2"/>
-    <row r="706" x14ac:dyDescent="0.2"/>
-    <row r="707" x14ac:dyDescent="0.2"/>
-    <row r="708" x14ac:dyDescent="0.2"/>
-    <row r="709" x14ac:dyDescent="0.2"/>
-    <row r="710" x14ac:dyDescent="0.2"/>
-    <row r="711" x14ac:dyDescent="0.2"/>
-    <row r="712" x14ac:dyDescent="0.2"/>
-    <row r="713" x14ac:dyDescent="0.2"/>
-    <row r="714" x14ac:dyDescent="0.2"/>
-    <row r="715" x14ac:dyDescent="0.2"/>
-    <row r="716" x14ac:dyDescent="0.2"/>
-    <row r="717" x14ac:dyDescent="0.2"/>
-    <row r="718" x14ac:dyDescent="0.2"/>
-    <row r="719" x14ac:dyDescent="0.2"/>
-    <row r="720" x14ac:dyDescent="0.2"/>
-    <row r="721" x14ac:dyDescent="0.2"/>
-    <row r="722" x14ac:dyDescent="0.2"/>
-    <row r="723" x14ac:dyDescent="0.2"/>
-    <row r="724" x14ac:dyDescent="0.2"/>
-    <row r="725" x14ac:dyDescent="0.2"/>
-    <row r="726" x14ac:dyDescent="0.2"/>
-    <row r="727" x14ac:dyDescent="0.2"/>
-    <row r="728" x14ac:dyDescent="0.2"/>
-    <row r="729" x14ac:dyDescent="0.2"/>
-    <row r="730" x14ac:dyDescent="0.2"/>
-    <row r="731" x14ac:dyDescent="0.2"/>
-    <row r="732" x14ac:dyDescent="0.2"/>
-    <row r="733" x14ac:dyDescent="0.2"/>
-    <row r="734" x14ac:dyDescent="0.2"/>
-    <row r="735" x14ac:dyDescent="0.2"/>
-    <row r="736" x14ac:dyDescent="0.2"/>
-    <row r="737" x14ac:dyDescent="0.2"/>
-    <row r="738" x14ac:dyDescent="0.2"/>
-    <row r="739" x14ac:dyDescent="0.2"/>
-    <row r="740" x14ac:dyDescent="0.2"/>
-    <row r="741" x14ac:dyDescent="0.2"/>
-    <row r="742" x14ac:dyDescent="0.2"/>
-    <row r="743" x14ac:dyDescent="0.2"/>
-    <row r="744" x14ac:dyDescent="0.2"/>
-    <row r="745" x14ac:dyDescent="0.2"/>
-    <row r="746" x14ac:dyDescent="0.2"/>
-    <row r="747" x14ac:dyDescent="0.2"/>
-    <row r="748" x14ac:dyDescent="0.2"/>
-    <row r="749" x14ac:dyDescent="0.2"/>
-    <row r="750" x14ac:dyDescent="0.2"/>
-    <row r="751" x14ac:dyDescent="0.2"/>
-    <row r="752" x14ac:dyDescent="0.2"/>
-    <row r="753" x14ac:dyDescent="0.2"/>
-    <row r="754" x14ac:dyDescent="0.2"/>
-    <row r="755" x14ac:dyDescent="0.2"/>
-    <row r="756" x14ac:dyDescent="0.2"/>
-    <row r="757" x14ac:dyDescent="0.2"/>
-    <row r="758" x14ac:dyDescent="0.2"/>
-    <row r="759" x14ac:dyDescent="0.2"/>
-    <row r="760" x14ac:dyDescent="0.2"/>
-    <row r="761" x14ac:dyDescent="0.2"/>
-    <row r="762" x14ac:dyDescent="0.2"/>
-    <row r="763" x14ac:dyDescent="0.2"/>
-    <row r="764" x14ac:dyDescent="0.2"/>
-    <row r="765" x14ac:dyDescent="0.2"/>
-    <row r="766" x14ac:dyDescent="0.2"/>
-    <row r="767" x14ac:dyDescent="0.2"/>
-    <row r="768" x14ac:dyDescent="0.2"/>
-    <row r="769" x14ac:dyDescent="0.2"/>
-    <row r="770" x14ac:dyDescent="0.2"/>
-    <row r="771" x14ac:dyDescent="0.2"/>
-    <row r="772" x14ac:dyDescent="0.2"/>
-    <row r="773" x14ac:dyDescent="0.2"/>
-    <row r="774" x14ac:dyDescent="0.2"/>
-    <row r="775" x14ac:dyDescent="0.2"/>
-    <row r="776" x14ac:dyDescent="0.2"/>
-    <row r="777" x14ac:dyDescent="0.2"/>
-    <row r="778" x14ac:dyDescent="0.2"/>
-    <row r="779" x14ac:dyDescent="0.2"/>
-    <row r="780" x14ac:dyDescent="0.2"/>
-    <row r="781" x14ac:dyDescent="0.2"/>
-    <row r="782" x14ac:dyDescent="0.2"/>
-    <row r="783" x14ac:dyDescent="0.2"/>
-    <row r="784" x14ac:dyDescent="0.2"/>
-    <row r="785" x14ac:dyDescent="0.2"/>
-    <row r="786" x14ac:dyDescent="0.2"/>
-    <row r="787" x14ac:dyDescent="0.2"/>
-    <row r="788" x14ac:dyDescent="0.2"/>
-    <row r="789" x14ac:dyDescent="0.2"/>
-    <row r="790" x14ac:dyDescent="0.2"/>
-    <row r="791" x14ac:dyDescent="0.2"/>
-    <row r="792" x14ac:dyDescent="0.2"/>
-    <row r="793" x14ac:dyDescent="0.2"/>
-    <row r="794" x14ac:dyDescent="0.2"/>
-    <row r="795" x14ac:dyDescent="0.2"/>
-    <row r="796" x14ac:dyDescent="0.2"/>
-    <row r="797" x14ac:dyDescent="0.2"/>
-    <row r="798" x14ac:dyDescent="0.2"/>
-    <row r="799" x14ac:dyDescent="0.2"/>
-    <row r="800" x14ac:dyDescent="0.2"/>
-    <row r="801" x14ac:dyDescent="0.2"/>
-    <row r="802" x14ac:dyDescent="0.2"/>
-    <row r="803" x14ac:dyDescent="0.2"/>
-    <row r="804" x14ac:dyDescent="0.2"/>
-    <row r="805" x14ac:dyDescent="0.2"/>
-    <row r="806" x14ac:dyDescent="0.2"/>
-    <row r="807" x14ac:dyDescent="0.2"/>
-    <row r="808" x14ac:dyDescent="0.2"/>
-    <row r="809" x14ac:dyDescent="0.2"/>
-    <row r="810" x14ac:dyDescent="0.2"/>
-    <row r="811" x14ac:dyDescent="0.2"/>
-    <row r="812" x14ac:dyDescent="0.2"/>
-    <row r="813" x14ac:dyDescent="0.2"/>
-    <row r="814" x14ac:dyDescent="0.2"/>
-    <row r="815" x14ac:dyDescent="0.2"/>
-    <row r="816" x14ac:dyDescent="0.2"/>
-    <row r="817" x14ac:dyDescent="0.2"/>
-    <row r="818" x14ac:dyDescent="0.2"/>
-    <row r="819" x14ac:dyDescent="0.2"/>
-    <row r="820" x14ac:dyDescent="0.2"/>
-    <row r="821" x14ac:dyDescent="0.2"/>
-    <row r="822" x14ac:dyDescent="0.2"/>
-    <row r="823" x14ac:dyDescent="0.2"/>
-    <row r="824" x14ac:dyDescent="0.2"/>
-    <row r="825" x14ac:dyDescent="0.2"/>
-    <row r="826" x14ac:dyDescent="0.2"/>
-    <row r="827" x14ac:dyDescent="0.2"/>
-    <row r="828" x14ac:dyDescent="0.2"/>
-    <row r="829" x14ac:dyDescent="0.2"/>
-    <row r="830" x14ac:dyDescent="0.2"/>
-    <row r="831" x14ac:dyDescent="0.2"/>
-    <row r="832" x14ac:dyDescent="0.2"/>
-    <row r="833" x14ac:dyDescent="0.2"/>
-    <row r="834" x14ac:dyDescent="0.2"/>
-    <row r="835" x14ac:dyDescent="0.2"/>
-    <row r="836" x14ac:dyDescent="0.2"/>
-    <row r="837" x14ac:dyDescent="0.2"/>
-    <row r="838" x14ac:dyDescent="0.2"/>
-    <row r="839" x14ac:dyDescent="0.2"/>
-    <row r="840" x14ac:dyDescent="0.2"/>
-    <row r="841" x14ac:dyDescent="0.2"/>
-    <row r="842" x14ac:dyDescent="0.2"/>
-    <row r="843" x14ac:dyDescent="0.2"/>
-    <row r="844" x14ac:dyDescent="0.2"/>
-    <row r="845" x14ac:dyDescent="0.2"/>
-    <row r="846" x14ac:dyDescent="0.2"/>
-    <row r="847" x14ac:dyDescent="0.2"/>
-    <row r="848" x14ac:dyDescent="0.2"/>
-    <row r="849" x14ac:dyDescent="0.2"/>
-    <row r="850" x14ac:dyDescent="0.2"/>
-    <row r="851" x14ac:dyDescent="0.2"/>
-    <row r="852" x14ac:dyDescent="0.2"/>
-    <row r="853" x14ac:dyDescent="0.2"/>
-    <row r="854" x14ac:dyDescent="0.2"/>
-    <row r="855" x14ac:dyDescent="0.2"/>
-    <row r="856" x14ac:dyDescent="0.2"/>
-    <row r="857" x14ac:dyDescent="0.2"/>
-    <row r="858" x14ac:dyDescent="0.2"/>
-    <row r="859" x14ac:dyDescent="0.2"/>
-    <row r="860" x14ac:dyDescent="0.2"/>
-    <row r="861" x14ac:dyDescent="0.2"/>
-    <row r="862" x14ac:dyDescent="0.2"/>
-    <row r="863" x14ac:dyDescent="0.2"/>
-    <row r="864" x14ac:dyDescent="0.2"/>
-    <row r="865" x14ac:dyDescent="0.2"/>
-    <row r="866" x14ac:dyDescent="0.2"/>
-    <row r="867" x14ac:dyDescent="0.2"/>
-    <row r="868" x14ac:dyDescent="0.2"/>
-    <row r="869" x14ac:dyDescent="0.2"/>
-    <row r="870" x14ac:dyDescent="0.2"/>
-    <row r="871" x14ac:dyDescent="0.2"/>
-    <row r="872" x14ac:dyDescent="0.2"/>
-    <row r="873" x14ac:dyDescent="0.2"/>
-    <row r="874" x14ac:dyDescent="0.2"/>
-    <row r="875" x14ac:dyDescent="0.2"/>
-    <row r="876" x14ac:dyDescent="0.2"/>
-    <row r="877" x14ac:dyDescent="0.2"/>
-    <row r="878" x14ac:dyDescent="0.2"/>
-    <row r="879" x14ac:dyDescent="0.2"/>
-    <row r="880" x14ac:dyDescent="0.2"/>
-    <row r="881" x14ac:dyDescent="0.2"/>
-    <row r="882" x14ac:dyDescent="0.2"/>
-    <row r="883" x14ac:dyDescent="0.2"/>
-    <row r="884" x14ac:dyDescent="0.2"/>
-    <row r="885" x14ac:dyDescent="0.2"/>
-    <row r="886" x14ac:dyDescent="0.2"/>
-    <row r="887" x14ac:dyDescent="0.2"/>
-    <row r="888" x14ac:dyDescent="0.2"/>
-    <row r="889" x14ac:dyDescent="0.2"/>
-    <row r="890" x14ac:dyDescent="0.2"/>
-    <row r="891" x14ac:dyDescent="0.2"/>
-    <row r="892" x14ac:dyDescent="0.2"/>
-    <row r="893" x14ac:dyDescent="0.2"/>
-    <row r="894" x14ac:dyDescent="0.2"/>
-    <row r="895" x14ac:dyDescent="0.2"/>
-    <row r="896" x14ac:dyDescent="0.2"/>
-    <row r="897" x14ac:dyDescent="0.2"/>
-    <row r="898" x14ac:dyDescent="0.2"/>
-    <row r="899" x14ac:dyDescent="0.2"/>
-    <row r="900" x14ac:dyDescent="0.2"/>
-    <row r="901" x14ac:dyDescent="0.2"/>
-    <row r="902" x14ac:dyDescent="0.2"/>
-    <row r="903" x14ac:dyDescent="0.2"/>
-    <row r="904" x14ac:dyDescent="0.2"/>
-    <row r="905" x14ac:dyDescent="0.2"/>
-    <row r="906" x14ac:dyDescent="0.2"/>
-    <row r="907" x14ac:dyDescent="0.2"/>
-    <row r="908" x14ac:dyDescent="0.2"/>
-    <row r="909" x14ac:dyDescent="0.2"/>
-    <row r="910" x14ac:dyDescent="0.2"/>
-    <row r="911" x14ac:dyDescent="0.2"/>
-    <row r="912" x14ac:dyDescent="0.2"/>
-    <row r="913" x14ac:dyDescent="0.2"/>
-    <row r="914" x14ac:dyDescent="0.2"/>
-    <row r="915" x14ac:dyDescent="0.2"/>
-    <row r="916" x14ac:dyDescent="0.2"/>
-    <row r="917" x14ac:dyDescent="0.2"/>
-    <row r="918" x14ac:dyDescent="0.2"/>
-    <row r="919" x14ac:dyDescent="0.2"/>
-    <row r="920" x14ac:dyDescent="0.2"/>
-    <row r="921" x14ac:dyDescent="0.2"/>
-    <row r="922" x14ac:dyDescent="0.2"/>
-    <row r="923" x14ac:dyDescent="0.2"/>
-    <row r="924" x14ac:dyDescent="0.2"/>
-    <row r="925" x14ac:dyDescent="0.2"/>
-    <row r="926" x14ac:dyDescent="0.2"/>
-    <row r="927" x14ac:dyDescent="0.2"/>
-    <row r="928" x14ac:dyDescent="0.2"/>
-    <row r="929" x14ac:dyDescent="0.2"/>
-    <row r="930" x14ac:dyDescent="0.2"/>
-    <row r="931" x14ac:dyDescent="0.2"/>
-    <row r="932" x14ac:dyDescent="0.2"/>
-    <row r="933" x14ac:dyDescent="0.2"/>
-    <row r="934" x14ac:dyDescent="0.2"/>
-    <row r="935" x14ac:dyDescent="0.2"/>
-    <row r="936" x14ac:dyDescent="0.2"/>
-    <row r="937" x14ac:dyDescent="0.2"/>
-    <row r="938" x14ac:dyDescent="0.2"/>
-    <row r="939" x14ac:dyDescent="0.2"/>
-    <row r="940" x14ac:dyDescent="0.2"/>
-    <row r="941" x14ac:dyDescent="0.2"/>
-    <row r="942" x14ac:dyDescent="0.2"/>
-    <row r="943" x14ac:dyDescent="0.2"/>
-    <row r="944" x14ac:dyDescent="0.2"/>
-    <row r="945" x14ac:dyDescent="0.2"/>
-    <row r="946" x14ac:dyDescent="0.2"/>
-    <row r="947" x14ac:dyDescent="0.2"/>
-    <row r="948" x14ac:dyDescent="0.2"/>
-    <row r="949" x14ac:dyDescent="0.2"/>
-    <row r="950" x14ac:dyDescent="0.2"/>
-    <row r="951" x14ac:dyDescent="0.2"/>
-    <row r="952" x14ac:dyDescent="0.2"/>
-    <row r="953" x14ac:dyDescent="0.2"/>
-    <row r="954" x14ac:dyDescent="0.2"/>
-    <row r="955" x14ac:dyDescent="0.2"/>
-    <row r="956" x14ac:dyDescent="0.2"/>
-    <row r="957" x14ac:dyDescent="0.2"/>
-    <row r="958" x14ac:dyDescent="0.2"/>
-    <row r="959" x14ac:dyDescent="0.2"/>
-    <row r="960" x14ac:dyDescent="0.2"/>
-    <row r="961" x14ac:dyDescent="0.2"/>
-    <row r="962" x14ac:dyDescent="0.2"/>
-    <row r="963" x14ac:dyDescent="0.2"/>
-    <row r="964" x14ac:dyDescent="0.2"/>
-    <row r="965" x14ac:dyDescent="0.2"/>
-    <row r="966" x14ac:dyDescent="0.2"/>
-    <row r="967" x14ac:dyDescent="0.2"/>
-    <row r="968" x14ac:dyDescent="0.2"/>
-    <row r="969" x14ac:dyDescent="0.2"/>
-    <row r="970" x14ac:dyDescent="0.2"/>
-    <row r="971" x14ac:dyDescent="0.2"/>
-    <row r="972" x14ac:dyDescent="0.2"/>
-    <row r="973" x14ac:dyDescent="0.2"/>
-    <row r="974" x14ac:dyDescent="0.2"/>
-    <row r="975" x14ac:dyDescent="0.2"/>
-    <row r="976" x14ac:dyDescent="0.2"/>
-    <row r="977" x14ac:dyDescent="0.2"/>
-    <row r="978" x14ac:dyDescent="0.2"/>
-    <row r="979" x14ac:dyDescent="0.2"/>
-    <row r="980" x14ac:dyDescent="0.2"/>
-    <row r="981" x14ac:dyDescent="0.2"/>
-    <row r="982" x14ac:dyDescent="0.2"/>
-    <row r="983" x14ac:dyDescent="0.2"/>
-    <row r="984" x14ac:dyDescent="0.2"/>
-    <row r="985" x14ac:dyDescent="0.2"/>
-    <row r="986" x14ac:dyDescent="0.2"/>
-    <row r="987" x14ac:dyDescent="0.2"/>
-    <row r="988" x14ac:dyDescent="0.2"/>
-    <row r="989" x14ac:dyDescent="0.2"/>
-    <row r="990" x14ac:dyDescent="0.2"/>
-    <row r="991" x14ac:dyDescent="0.2"/>
-    <row r="992" x14ac:dyDescent="0.2"/>
-    <row r="993" x14ac:dyDescent="0.2"/>
-    <row r="994" x14ac:dyDescent="0.2"/>
-    <row r="995" x14ac:dyDescent="0.2"/>
-    <row r="996" x14ac:dyDescent="0.2"/>
-    <row r="997" x14ac:dyDescent="0.2"/>
-    <row r="998" x14ac:dyDescent="0.2"/>
-    <row r="999" x14ac:dyDescent="0.2"/>
-    <row r="1000" x14ac:dyDescent="0.2"/>
-    <row r="1001" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>